<commit_message>
ultimate gage 기획대로 damage 마다 적용
</commit_message>
<xml_diff>
--- a/Assets/04Table/TS.xlsx
+++ b/Assets/04Table/TS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cksgm\Unity\ProjectTS\Assets\04Table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B264DA65-B220-4236-8DBA-B559AAB75E0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{564AEDB3-8053-4470-90BD-0C17692AE164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1585,8 +1585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AC183E9-B7A8-46E9-9BBC-B44B6B1E4A99}">
   <dimension ref="A1:P86"/>
   <sheetViews>
-    <sheetView topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="S83" sqref="S83"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="J78" sqref="J78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17"/>
@@ -5992,13 +5992,13 @@
         <v>201</v>
       </c>
       <c r="B4" s="6">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C4" s="6">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D4" s="6">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E4" s="6">
         <v>0</v>

</xml_diff>

<commit_message>
PIN POINT DOWN 진행 중
</commit_message>
<xml_diff>
--- a/Assets/04Table/TS.xlsx
+++ b/Assets/04Table/TS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cksgm\Unity\ProjectTS\Assets\04Table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE565B9F-8E54-4484-8F2B-AE734C22AAE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC05EF05-77DC-4DAD-9247-F0057DCF9399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="400" windowWidth="22110" windowHeight="13280" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="127">
   <si>
     <t>Level</t>
   </si>
@@ -451,6 +451,9 @@
   <si>
     <t>Scoping_Time</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Linked_Skill</t>
   </si>
 </sst>
 </file>
@@ -826,7 +829,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -959,6 +962,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1406,10 +1412,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2F9EEC3-3347-4F2E-9FD6-D990126A68DE}">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="M1" sqref="M1:M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="17"/>
@@ -1424,7 +1430,7 @@
     <col min="11" max="16384" width="8.58203125" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="34.5" thickBot="1">
+    <row r="1" spans="1:13" ht="34.5" thickBot="1">
       <c r="A1" s="8" t="s">
         <v>15</v>
       </c>
@@ -1461,8 +1467,11 @@
       <c r="L1" s="25" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="34.5" thickBot="1">
+      <c r="M1" s="47" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="34.5" thickBot="1">
       <c r="A2" s="6">
         <v>100</v>
       </c>
@@ -1499,8 +1508,11 @@
       <c r="L2" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="34.5" thickBot="1">
+      <c r="M2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="34.5" thickBot="1">
       <c r="A3" s="6">
         <v>101</v>
       </c>
@@ -1537,8 +1549,11 @@
       <c r="L3" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="17.5" thickBot="1">
+      <c r="M3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="17.5" thickBot="1">
       <c r="A4" s="24">
         <v>102</v>
       </c>
@@ -1575,8 +1590,11 @@
       <c r="L4" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="17.5" thickBot="1">
+      <c r="M4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="17.5" thickBot="1">
       <c r="A5" s="6">
         <v>103</v>
       </c>
@@ -1613,8 +1631,11 @@
       <c r="L5" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="17.5" thickBot="1">
+      <c r="M5" s="1">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="17.5" thickBot="1">
       <c r="A6" s="6">
         <v>104</v>
       </c>
@@ -1651,8 +1672,11 @@
       <c r="L6" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="34.5" thickBot="1">
+      <c r="M6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="34.5" thickBot="1">
       <c r="A7" s="6">
         <v>200</v>
       </c>
@@ -1689,8 +1713,11 @@
       <c r="L7" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="34.5" thickBot="1">
+      <c r="M7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="34.5" thickBot="1">
       <c r="A8" s="6">
         <v>201</v>
       </c>
@@ -1727,8 +1754,11 @@
       <c r="L8" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="17.5" thickBot="1">
+      <c r="M8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="17.5" thickBot="1">
       <c r="A9" s="6">
         <v>202</v>
       </c>
@@ -1765,8 +1795,11 @@
       <c r="L9" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="17.5" thickBot="1">
+      <c r="M9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="17.5" thickBot="1">
       <c r="A10" s="6">
         <v>203</v>
       </c>
@@ -1803,8 +1836,11 @@
       <c r="L10" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="17.5" thickBot="1">
+      <c r="M10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="17.5" thickBot="1">
       <c r="A11" s="6">
         <v>231</v>
       </c>
@@ -1841,8 +1877,11 @@
       <c r="L11" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="17.5" thickBot="1">
+      <c r="M11" s="1">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="17.5" thickBot="1">
       <c r="A12" s="6">
         <v>232</v>
       </c>
@@ -1879,8 +1918,11 @@
       <c r="L12" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="17.5" thickBot="1">
+      <c r="M12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="17.5" thickBot="1">
       <c r="A13" s="6">
         <v>300</v>
       </c>
@@ -1917,8 +1959,11 @@
       <c r="L13" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="17.5" thickBot="1">
+      <c r="M13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="17.5" thickBot="1">
       <c r="A14" s="6">
         <v>301</v>
       </c>
@@ -1955,8 +2000,11 @@
       <c r="L14" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="17.5" thickBot="1">
+      <c r="M14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="17.5" thickBot="1">
       <c r="A15" s="6">
         <v>302</v>
       </c>
@@ -1993,8 +2041,11 @@
       <c r="L15" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" ht="34.5" thickBot="1">
+      <c r="M15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="34.5" thickBot="1">
       <c r="A16" s="6">
         <v>303</v>
       </c>
@@ -2031,8 +2082,11 @@
       <c r="L16" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" ht="17.5" thickBot="1">
+      <c r="M16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="17.5" thickBot="1">
       <c r="A17" s="6">
         <v>331</v>
       </c>
@@ -2067,6 +2121,9 @@
         <v>0</v>
       </c>
       <c r="L17" s="6">
+        <v>0</v>
+      </c>
+      <c r="M17" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cool time 1,  hit effect, TestScene
</commit_message>
<xml_diff>
--- a/Assets/04Table/TS.xlsx
+++ b/Assets/04Table/TS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cksgm\Unity\ProjectTS\Assets\04Table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6291604-B650-4D90-B6E9-F68D8C41FEE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56F9761-4B1D-4885-AA04-57769330211E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="400" windowWidth="22110" windowHeight="13280" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2171,8 +2171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AC183E9-B7A8-46E9-9BBC-B44B6B1E4A99}">
   <dimension ref="A1:Z136"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3:K136"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="K118" sqref="K118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="17"/>
@@ -2363,7 +2363,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4" s="6">
         <v>0</v>
@@ -2413,7 +2413,7 @@
         <v>0</v>
       </c>
       <c r="K5" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5" s="6">
         <v>0</v>
@@ -2463,7 +2463,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6" s="6">
         <v>0</v>
@@ -2513,7 +2513,7 @@
         <v>0</v>
       </c>
       <c r="K7" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7" s="6">
         <v>0</v>
@@ -2563,7 +2563,7 @@
         <v>0</v>
       </c>
       <c r="K8" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8" s="6">
         <v>0</v>
@@ -2613,7 +2613,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9" s="6">
         <v>0</v>
@@ -2663,7 +2663,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10" s="6">
         <v>0</v>
@@ -2713,7 +2713,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11" s="6">
         <v>0</v>
@@ -2763,7 +2763,7 @@
         <v>0</v>
       </c>
       <c r="K12" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L12" s="6">
         <v>0</v>
@@ -2813,7 +2813,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L13" s="6">
         <v>0</v>
@@ -2863,7 +2863,7 @@
         <v>0</v>
       </c>
       <c r="K14" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14" s="34">
         <v>0</v>
@@ -2913,7 +2913,7 @@
         <v>0</v>
       </c>
       <c r="K15" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15" s="37">
         <v>0</v>
@@ -2963,7 +2963,7 @@
         <v>0</v>
       </c>
       <c r="K16" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16" s="37">
         <v>0</v>
@@ -3013,7 +3013,7 @@
         <v>0</v>
       </c>
       <c r="K17" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17" s="37">
         <v>0</v>
@@ -3063,7 +3063,7 @@
         <v>0</v>
       </c>
       <c r="K18" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L18" s="37">
         <v>0</v>
@@ -3113,7 +3113,7 @@
         <v>0</v>
       </c>
       <c r="K19" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L19" s="37">
         <v>0</v>
@@ -3163,7 +3163,7 @@
         <v>0</v>
       </c>
       <c r="K20" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L20" s="37">
         <v>0</v>
@@ -3213,7 +3213,7 @@
         <v>0</v>
       </c>
       <c r="K21" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L21" s="37">
         <v>0</v>
@@ -3263,7 +3263,7 @@
         <v>0</v>
       </c>
       <c r="K22" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L22" s="37">
         <v>0</v>
@@ -3313,7 +3313,7 @@
         <v>0</v>
       </c>
       <c r="K23" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L23" s="37">
         <v>0</v>
@@ -3363,7 +3363,7 @@
         <v>0</v>
       </c>
       <c r="K24" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L24" s="37">
         <v>0</v>
@@ -3413,7 +3413,7 @@
         <v>0</v>
       </c>
       <c r="K25" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L25" s="37">
         <v>0</v>
@@ -3463,7 +3463,7 @@
         <v>0</v>
       </c>
       <c r="K26" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L26" s="37">
         <v>0</v>
@@ -3513,7 +3513,7 @@
         <v>0</v>
       </c>
       <c r="K27" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L27" s="37">
         <v>0</v>
@@ -3563,7 +3563,7 @@
         <v>0</v>
       </c>
       <c r="K28" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L28" s="40">
         <v>0</v>
@@ -3613,7 +3613,7 @@
         <v>0</v>
       </c>
       <c r="K29" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L29" s="6">
         <v>0</v>
@@ -3663,7 +3663,7 @@
         <v>0</v>
       </c>
       <c r="K30" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L30" s="6">
         <v>0</v>
@@ -3713,7 +3713,7 @@
         <v>0</v>
       </c>
       <c r="K31" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L31" s="6">
         <v>0</v>
@@ -3763,7 +3763,7 @@
         <v>0</v>
       </c>
       <c r="K32" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L32" s="6">
         <v>0</v>
@@ -3813,7 +3813,7 @@
         <v>0</v>
       </c>
       <c r="K33" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L33" s="6">
         <v>0</v>
@@ -3863,7 +3863,7 @@
         <v>0</v>
       </c>
       <c r="K34" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L34" s="6">
         <v>0</v>
@@ -3913,7 +3913,7 @@
         <v>0</v>
       </c>
       <c r="K35" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L35" s="6">
         <v>0</v>
@@ -3963,7 +3963,7 @@
         <v>0</v>
       </c>
       <c r="K36" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L36" s="6">
         <v>0</v>
@@ -4013,7 +4013,7 @@
         <v>0</v>
       </c>
       <c r="K37" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L37" s="6">
         <v>0</v>
@@ -4063,7 +4063,7 @@
         <v>0</v>
       </c>
       <c r="K38" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L38" s="6">
         <v>0</v>
@@ -4113,7 +4113,7 @@
         <v>0</v>
       </c>
       <c r="K39" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L39" s="6">
         <v>0</v>
@@ -4163,7 +4163,7 @@
         <v>0</v>
       </c>
       <c r="K40" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L40" s="6">
         <v>0</v>
@@ -4213,7 +4213,7 @@
         <v>0</v>
       </c>
       <c r="K41" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L41" s="6">
         <v>0</v>
@@ -4263,7 +4263,7 @@
         <v>0</v>
       </c>
       <c r="K42" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L42" s="6">
         <v>0</v>
@@ -4313,7 +4313,7 @@
         <v>0</v>
       </c>
       <c r="K43" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L43" s="6">
         <v>0</v>
@@ -4363,7 +4363,7 @@
         <v>0</v>
       </c>
       <c r="K44" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L44" s="6">
         <v>0</v>
@@ -4413,7 +4413,7 @@
         <v>0</v>
       </c>
       <c r="K45" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L45" s="6">
         <v>0</v>
@@ -4463,7 +4463,7 @@
         <v>0</v>
       </c>
       <c r="K46" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L46" s="6">
         <v>0</v>
@@ -4513,7 +4513,7 @@
         <v>0</v>
       </c>
       <c r="K47" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L47" s="6">
         <v>0</v>
@@ -4563,7 +4563,7 @@
         <v>0</v>
       </c>
       <c r="K48" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L48" s="6">
         <v>0</v>
@@ -4613,7 +4613,7 @@
         <v>0</v>
       </c>
       <c r="K49" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L49" s="6">
         <v>120000</v>
@@ -4673,7 +4673,7 @@
         <v>0</v>
       </c>
       <c r="K50" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L50" s="6">
         <v>110000</v>
@@ -4733,7 +4733,7 @@
         <v>0</v>
       </c>
       <c r="K51" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L51" s="6">
         <v>100000</v>
@@ -4893,7 +4893,7 @@
         <v>0</v>
       </c>
       <c r="K54" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L54" s="6">
         <v>0</v>
@@ -4943,7 +4943,7 @@
         <v>0</v>
       </c>
       <c r="K55" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L55" s="6">
         <v>0</v>
@@ -4993,7 +4993,7 @@
         <v>0</v>
       </c>
       <c r="K56" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L56" s="6">
         <v>0</v>
@@ -5043,7 +5043,7 @@
         <v>0</v>
       </c>
       <c r="K57" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L57" s="6">
         <v>0</v>
@@ -5093,7 +5093,7 @@
         <v>0</v>
       </c>
       <c r="K58" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L58" s="6">
         <v>0</v>
@@ -5143,7 +5143,7 @@
         <v>0</v>
       </c>
       <c r="K59" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L59" s="6">
         <v>0</v>
@@ -5193,7 +5193,7 @@
         <v>0</v>
       </c>
       <c r="K60" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L60" s="6">
         <v>0</v>
@@ -5243,7 +5243,7 @@
         <v>0</v>
       </c>
       <c r="K61" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L61" s="6">
         <v>0</v>
@@ -5293,7 +5293,7 @@
         <v>0</v>
       </c>
       <c r="K62" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L62" s="6">
         <v>0</v>
@@ -5343,7 +5343,7 @@
         <v>0</v>
       </c>
       <c r="K63" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L63" s="6">
         <v>0</v>
@@ -5393,7 +5393,7 @@
         <v>0</v>
       </c>
       <c r="K64" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L64" s="6">
         <v>0</v>
@@ -5443,7 +5443,7 @@
         <v>10</v>
       </c>
       <c r="K65" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L65" s="6">
         <v>0</v>
@@ -5493,7 +5493,7 @@
         <v>0</v>
       </c>
       <c r="K66" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L66" s="6">
         <v>0</v>
@@ -5543,7 +5543,7 @@
         <v>10</v>
       </c>
       <c r="K67" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L67" s="6">
         <v>0</v>
@@ -5593,7 +5593,7 @@
         <v>0</v>
       </c>
       <c r="K68" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L68" s="6">
         <v>0</v>
@@ -5643,7 +5643,7 @@
         <v>10</v>
       </c>
       <c r="K69" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L69" s="6">
         <v>0</v>
@@ -5693,7 +5693,7 @@
         <v>0</v>
       </c>
       <c r="K70" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L70" s="6">
         <v>0</v>
@@ -5743,7 +5743,7 @@
         <v>10</v>
       </c>
       <c r="K71" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L71" s="6">
         <v>0</v>
@@ -5793,7 +5793,7 @@
         <v>0</v>
       </c>
       <c r="K72" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L72" s="6">
         <v>0</v>
@@ -5843,7 +5843,7 @@
         <v>10</v>
       </c>
       <c r="K73" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L73" s="6">
         <v>0</v>
@@ -5893,7 +5893,7 @@
         <v>0</v>
       </c>
       <c r="K74" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L74" s="6">
         <v>0</v>
@@ -5943,7 +5943,7 @@
         <v>10</v>
       </c>
       <c r="K75" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L75" s="6">
         <v>0</v>
@@ -5993,7 +5993,7 @@
         <v>10</v>
       </c>
       <c r="K76" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L76" s="6">
         <v>0</v>
@@ -6043,7 +6043,7 @@
         <v>0</v>
       </c>
       <c r="K77" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L77" s="6">
         <v>0</v>
@@ -6093,7 +6093,7 @@
         <v>10</v>
       </c>
       <c r="K78" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L78" s="6">
         <v>0</v>
@@ -6143,7 +6143,7 @@
         <v>10</v>
       </c>
       <c r="K79" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L79" s="6">
         <v>0</v>
@@ -6193,7 +6193,7 @@
         <v>0</v>
       </c>
       <c r="K80" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L80" s="6">
         <v>0</v>
@@ -6243,7 +6243,7 @@
         <v>10</v>
       </c>
       <c r="K81" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L81" s="6">
         <v>0</v>
@@ -6293,7 +6293,7 @@
         <v>10</v>
       </c>
       <c r="K82" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L82" s="6">
         <v>0</v>
@@ -6343,7 +6343,7 @@
         <v>0</v>
       </c>
       <c r="K83" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L83" s="6">
         <v>0</v>
@@ -6393,7 +6393,7 @@
         <v>10</v>
       </c>
       <c r="K84" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L84" s="6">
         <v>0</v>
@@ -6443,7 +6443,7 @@
         <v>10</v>
       </c>
       <c r="K85" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L85" s="6">
         <v>0</v>
@@ -6493,7 +6493,7 @@
         <v>0</v>
       </c>
       <c r="K86" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L86" s="6">
         <v>0</v>
@@ -6543,7 +6543,7 @@
         <v>10</v>
       </c>
       <c r="K87" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L87" s="6">
         <v>0</v>
@@ -6593,7 +6593,7 @@
         <v>10</v>
       </c>
       <c r="K88" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L88" s="6">
         <v>0</v>
@@ -6643,7 +6643,7 @@
         <v>0</v>
       </c>
       <c r="K89" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L89" s="6">
         <v>0</v>
@@ -6693,7 +6693,7 @@
         <v>0</v>
       </c>
       <c r="K90" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L90" s="6">
         <v>0</v>
@@ -6743,7 +6743,7 @@
         <v>0</v>
       </c>
       <c r="K91" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L91" s="6">
         <v>0</v>
@@ -6793,7 +6793,7 @@
         <v>0</v>
       </c>
       <c r="K92" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L92" s="6">
         <v>0</v>
@@ -6843,7 +6843,7 @@
         <v>0</v>
       </c>
       <c r="K93" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L93" s="6">
         <v>0</v>
@@ -6893,7 +6893,7 @@
         <v>0</v>
       </c>
       <c r="K94" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L94" s="6">
         <v>0</v>
@@ -6943,7 +6943,7 @@
         <v>0</v>
       </c>
       <c r="K95" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L95" s="6">
         <v>0</v>
@@ -6993,7 +6993,7 @@
         <v>0</v>
       </c>
       <c r="K96" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L96" s="6">
         <v>0</v>
@@ -7043,7 +7043,7 @@
         <v>0</v>
       </c>
       <c r="K97" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L97" s="6">
         <v>0</v>
@@ -7093,7 +7093,7 @@
         <v>0</v>
       </c>
       <c r="K98" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L98" s="6">
         <v>0</v>
@@ -7143,7 +7143,7 @@
         <v>0</v>
       </c>
       <c r="K99" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L99" s="6">
         <v>0</v>
@@ -7193,7 +7193,7 @@
         <v>0</v>
       </c>
       <c r="K100" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L100" s="6">
         <v>0</v>
@@ -7243,7 +7243,7 @@
         <v>0</v>
       </c>
       <c r="K101" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L101" s="6">
         <v>0</v>
@@ -7293,7 +7293,7 @@
         <v>0</v>
       </c>
       <c r="K102" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L102" s="6">
         <v>0</v>
@@ -7343,7 +7343,7 @@
         <v>0</v>
       </c>
       <c r="K103" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L103" s="6">
         <v>0</v>
@@ -7393,7 +7393,7 @@
         <v>0</v>
       </c>
       <c r="K104" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L104" s="6">
         <v>0</v>
@@ -7443,7 +7443,7 @@
         <v>0</v>
       </c>
       <c r="K105" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L105" s="6">
         <v>0</v>
@@ -7493,7 +7493,7 @@
         <v>0</v>
       </c>
       <c r="K106" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L106" s="6">
         <v>0</v>
@@ -7543,7 +7543,7 @@
         <v>0</v>
       </c>
       <c r="K107" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L107" s="6">
         <v>0</v>
@@ -7593,7 +7593,7 @@
         <v>0</v>
       </c>
       <c r="K108" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L108" s="6">
         <v>0</v>
@@ -7643,7 +7643,7 @@
         <v>0</v>
       </c>
       <c r="K109" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L109" s="6">
         <v>60000</v>
@@ -7693,7 +7693,7 @@
         <v>0</v>
       </c>
       <c r="K110" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L110" s="6">
         <v>55000</v>
@@ -7743,7 +7743,7 @@
         <v>0</v>
       </c>
       <c r="K111" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L111" s="6">
         <v>50000</v>
@@ -7793,7 +7793,7 @@
         <v>0</v>
       </c>
       <c r="K112" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L112" s="6">
         <v>0</v>
@@ -7843,7 +7843,7 @@
         <v>0</v>
       </c>
       <c r="K113" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L113" s="6">
         <v>0</v>
@@ -7893,7 +7893,7 @@
         <v>0</v>
       </c>
       <c r="K114" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L114" s="6">
         <v>0</v>
@@ -7943,7 +7943,7 @@
         <v>0</v>
       </c>
       <c r="K115" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L115" s="6">
         <v>0</v>
@@ -7993,7 +7993,7 @@
         <v>0</v>
       </c>
       <c r="K116" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L116" s="6">
         <v>0</v>
@@ -8043,7 +8043,7 @@
         <v>0</v>
       </c>
       <c r="K117" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L117" s="6">
         <v>0</v>
@@ -8143,7 +8143,7 @@
         <v>0</v>
       </c>
       <c r="K119" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L119" s="6">
         <v>0</v>
@@ -8193,7 +8193,7 @@
         <v>0</v>
       </c>
       <c r="K120" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L120" s="6">
         <v>0</v>
@@ -8243,7 +8243,7 @@
         <v>0</v>
       </c>
       <c r="K121" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L121" s="6">
         <v>0</v>
@@ -8293,7 +8293,7 @@
         <v>0</v>
       </c>
       <c r="K122" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L122" s="6">
         <v>0</v>
@@ -8343,7 +8343,7 @@
         <v>0</v>
       </c>
       <c r="K123" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L123" s="6">
         <v>0</v>
@@ -8393,7 +8393,7 @@
         <v>0</v>
       </c>
       <c r="K124" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L124" s="6">
         <v>0</v>
@@ -8443,7 +8443,7 @@
         <v>0</v>
       </c>
       <c r="K125" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L125" s="6">
         <v>0</v>
@@ -8493,7 +8493,7 @@
         <v>0</v>
       </c>
       <c r="K126" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L126" s="6">
         <v>0</v>
@@ -8543,7 +8543,7 @@
         <v>0</v>
       </c>
       <c r="K127" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L127" s="6">
         <v>0</v>
@@ -8593,7 +8593,7 @@
         <v>0</v>
       </c>
       <c r="K128" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L128" s="6">
         <v>0</v>
@@ -8643,7 +8643,7 @@
         <v>0</v>
       </c>
       <c r="K129" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L129" s="6">
         <v>0</v>
@@ -8693,7 +8693,7 @@
         <v>0</v>
       </c>
       <c r="K130" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L130" s="6">
         <v>0</v>
@@ -8743,7 +8743,7 @@
         <v>0</v>
       </c>
       <c r="K131" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L131" s="6">
         <v>0</v>
@@ -8793,7 +8793,7 @@
         <v>0</v>
       </c>
       <c r="K132" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L132" s="6">
         <v>0</v>
@@ -8843,7 +8843,7 @@
         <v>0</v>
       </c>
       <c r="K133" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L133" s="6">
         <v>0</v>
@@ -8893,7 +8893,7 @@
         <v>0</v>
       </c>
       <c r="K134" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L134" s="6">
         <v>80000</v>
@@ -8943,7 +8943,7 @@
         <v>0</v>
       </c>
       <c r="K135" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L135" s="6">
         <v>70000</v>
@@ -8993,7 +8993,7 @@
         <v>0</v>
       </c>
       <c r="K136" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L136" s="6">
         <v>60000</v>

</xml_diff>

<commit_message>
Table Pattern 수정, PatternManager 생성, 총 궁극기 완성
</commit_message>
<xml_diff>
--- a/Assets/04Table/TS.xlsx
+++ b/Assets/04Table/TS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cksgm\Unity\ProjectTS\Assets\04Table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D406DF82-CC1C-4F60-8BDC-3BD8CD705116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8CFCC5A-F23D-4666-9D7F-05331377E02D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="400" windowWidth="20730" windowHeight="13280" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="750" yWindow="400" windowWidth="20730" windowHeight="13280" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Player_Stats" sheetId="1" r:id="rId1"/>
@@ -474,24 +474,6 @@
     <t>듀리노 일반 공격</t>
   </si>
   <si>
-    <t>Physics_A</t>
-  </si>
-  <si>
-    <t>Fire_A</t>
-  </si>
-  <si>
-    <t>Water_A</t>
-  </si>
-  <si>
-    <t>Electric_A</t>
-  </si>
-  <si>
-    <t>Ice_A</t>
-  </si>
-  <si>
-    <t>Wind_A</t>
-  </si>
-  <si>
     <t>Creature_ID</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -575,6 +557,30 @@
   </si>
   <si>
     <t>Wind_Def</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ice_Mul</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wind_Mul</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Electric_Mul</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Water_Mul</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fire_Mul</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Physics_Mul</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -10132,7 +10138,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CAA2E81-D44D-4A2E-AECA-D182B5D7BC40}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -10140,43 +10146,43 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B1" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C1" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D1" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G1" t="s">
         <v>154</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>155</v>
-      </c>
-      <c r="G1" t="s">
-        <v>160</v>
-      </c>
-      <c r="H1" t="s">
-        <v>161</v>
       </c>
       <c r="I1" t="s">
         <v>104</v>
       </c>
       <c r="J1" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="K1" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="L1" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="M1" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="N1" t="s">
         <v>109</v>
@@ -10236,7 +10242,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B4BE54-90AE-4DAF-BA80-4CA3867A9D82}">
   <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
@@ -10476,22 +10482,22 @@
         <v>15</v>
       </c>
       <c r="B1" s="55" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C1" s="56" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D1" s="57" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="E1" s="57" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="F1" s="58" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="G1" s="58" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="H1" s="58" t="s">
         <v>128</v>
@@ -10578,7 +10584,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17"/>
@@ -10595,40 +10601,40 @@
         <v>15</v>
       </c>
       <c r="B1" s="61" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C1" s="57" t="s">
-        <v>132</v>
+        <v>161</v>
       </c>
       <c r="D1" s="57" t="s">
-        <v>133</v>
+        <v>160</v>
       </c>
       <c r="E1" s="57" t="s">
-        <v>134</v>
+        <v>159</v>
       </c>
       <c r="F1" s="57" t="s">
-        <v>135</v>
+        <v>158</v>
       </c>
       <c r="G1" s="57" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="H1" s="57" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="I1" s="62" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="J1" s="56" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="K1" s="56" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="L1" s="56" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="M1" s="63" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="N1" s="18"/>
     </row>

</xml_diff>

<commit_message>
pinpoint down size fix
</commit_message>
<xml_diff>
--- a/Assets/04Table/TS.xlsx
+++ b/Assets/04Table/TS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GameSW\Documents\GitHub\ProjectTS\Assets\04Table\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cksgm\Unity\ProjectTS\Assets\04Table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF876620-B3E4-45F0-A7AB-724FCC56AA85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83C659C-F74D-4B3C-9624-2DE0467D73AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="750" yWindow="400" windowWidth="20730" windowHeight="13280" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Player_Stats" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="192">
   <si>
     <t>Level</t>
   </si>
@@ -661,6 +661,18 @@
   </si>
   <si>
     <t>Medical_Ship</t>
+  </si>
+  <si>
+    <t>카타안킬로 V2</t>
+  </si>
+  <si>
+    <t>카타안킬로 V3</t>
+  </si>
+  <si>
+    <t>듀리노 V2</t>
+  </si>
+  <si>
+    <t>Drop_Exp</t>
   </si>
 </sst>
 </file>
@@ -719,7 +731,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -807,6 +819,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA8D08D"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1029,7 +1047,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -1214,8 +1232,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1503,9 +1524,9 @@
       <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <sheetData>
-    <row r="1" spans="1:16" ht="50.25" thickBot="1">
+    <row r="1" spans="1:16" ht="51.5" thickBot="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1552,7 +1573,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="17.25" thickBot="1">
+    <row r="2" spans="1:16" ht="17.5" thickBot="1">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1600,59 +1621,59 @@
       </c>
       <c r="P2" s="5"/>
     </row>
-    <row r="3" spans="1:16" ht="17.25" thickBot="1">
+    <row r="3" spans="1:16" ht="17.5" thickBot="1">
       <c r="A3" s="4"/>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:16" ht="17.25" thickBot="1">
+    <row r="4" spans="1:16" ht="17.5" thickBot="1">
       <c r="A4" s="4"/>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:16" ht="17.25" thickBot="1">
+    <row r="5" spans="1:16" ht="17.5" thickBot="1">
       <c r="A5" s="4"/>
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:16" ht="17.25" thickBot="1">
+    <row r="6" spans="1:16" ht="17.5" thickBot="1">
       <c r="A6" s="4"/>
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:16" ht="17.25" thickBot="1">
+    <row r="7" spans="1:16" ht="17.5" thickBot="1">
       <c r="A7" s="4"/>
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:16" ht="17.25" thickBot="1">
+    <row r="8" spans="1:16" ht="17.5" thickBot="1">
       <c r="A8" s="4"/>
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:16" ht="17.25" thickBot="1">
+    <row r="9" spans="1:16" ht="17.5" thickBot="1">
       <c r="A9" s="4"/>
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:16" ht="17.25" thickBot="1">
+    <row r="10" spans="1:16" ht="17.5" thickBot="1">
       <c r="A10" s="4"/>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:16" ht="17.25" thickBot="1">
+    <row r="11" spans="1:16" ht="17.5" thickBot="1">
       <c r="A11" s="4"/>
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:16" ht="17.25" thickBot="1">
+    <row r="12" spans="1:16" ht="17.5" thickBot="1">
       <c r="A12" s="4"/>
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:16" ht="17.25" thickBot="1">
+    <row r="13" spans="1:16" ht="17.5" thickBot="1">
       <c r="A13" s="4"/>
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:16" ht="17.25" thickBot="1">
+    <row r="14" spans="1:16" ht="17.5" thickBot="1">
       <c r="A14" s="4"/>
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:16" ht="17.25" thickBot="1">
+    <row r="15" spans="1:16" ht="17.5" thickBot="1">
       <c r="A15" s="4"/>
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:16" ht="17.25" thickBot="1">
+    <row r="16" spans="1:16" ht="17.5" thickBot="1">
       <c r="A16" s="1"/>
     </row>
   </sheetData>
@@ -1669,9 +1690,9 @@
       <selection activeCell="G3" sqref="A1:G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.25" thickBot="1">
+    <row r="1" spans="1:7" ht="17.5" thickBot="1">
       <c r="A1" s="52" t="s">
         <v>15</v>
       </c>
@@ -1694,7 +1715,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="17.25" thickBot="1">
+    <row r="2" spans="1:7" ht="17.5" thickBot="1">
       <c r="A2" s="9">
         <v>100000</v>
       </c>
@@ -1717,7 +1738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="17.25" thickBot="1">
+    <row r="3" spans="1:7" ht="17.5" thickBot="1">
       <c r="A3" s="9">
         <v>200000</v>
       </c>
@@ -1750,23 +1771,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAE0AA7C-D827-478C-A8E1-4F3353839195}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="A1:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="13.25" customWidth="1"/>
-    <col min="2" max="2" width="11.375" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
     <col min="3" max="3" width="10.25" customWidth="1"/>
-    <col min="4" max="4" width="11.625" customWidth="1"/>
+    <col min="4" max="4" width="11.58203125" customWidth="1"/>
     <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.75" customWidth="1"/>
-    <col min="7" max="7" width="13.125" customWidth="1"/>
-    <col min="8" max="8" width="17.875" customWidth="1"/>
+    <col min="7" max="7" width="13.08203125" customWidth="1"/>
+    <col min="8" max="8" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17.25" thickBot="1">
+    <row r="1" spans="1:8" ht="17.5" thickBot="1">
       <c r="A1" s="18" t="s">
         <v>170</v>
       </c>
@@ -1792,7 +1813,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="33.75" thickBot="1">
+    <row r="2" spans="1:8" ht="34.5" thickBot="1">
       <c r="A2" s="18">
         <v>2</v>
       </c>
@@ -1818,7 +1839,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="33.75" thickBot="1">
+    <row r="3" spans="1:8" ht="34.5" thickBot="1">
       <c r="A3" s="18">
         <v>2</v>
       </c>
@@ -1844,7 +1865,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="33.75" thickBot="1">
+    <row r="4" spans="1:8" ht="34.5" thickBot="1">
       <c r="A4" s="18">
         <v>2</v>
       </c>
@@ -1870,7 +1891,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="33.75" thickBot="1">
+    <row r="5" spans="1:8" ht="34.5" thickBot="1">
       <c r="A5" s="18">
         <v>3</v>
       </c>
@@ -1896,7 +1917,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="33.75" thickBot="1">
+    <row r="6" spans="1:8" ht="34.5" thickBot="1">
       <c r="A6" s="18">
         <v>3</v>
       </c>
@@ -1922,7 +1943,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="33.75" thickBot="1">
+    <row r="7" spans="1:8" ht="17.5" thickBot="1">
       <c r="A7" s="18">
         <v>3</v>
       </c>
@@ -1963,19 +1984,19 @@
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="8.625" style="18"/>
-    <col min="2" max="2" width="14.375" style="18" customWidth="1"/>
-    <col min="3" max="6" width="8.625" style="18"/>
+    <col min="1" max="1" width="8.58203125" style="18"/>
+    <col min="2" max="2" width="14.33203125" style="18" customWidth="1"/>
+    <col min="3" max="6" width="8.58203125" style="18"/>
     <col min="7" max="7" width="10.5" style="18" customWidth="1"/>
-    <col min="8" max="8" width="21.625" style="18" customWidth="1"/>
-    <col min="9" max="9" width="8.625" style="18"/>
+    <col min="8" max="8" width="21.58203125" style="18" customWidth="1"/>
+    <col min="9" max="9" width="8.58203125" style="18"/>
     <col min="10" max="10" width="13.75" style="18" customWidth="1"/>
-    <col min="11" max="16384" width="8.625" style="18"/>
+    <col min="11" max="16384" width="8.58203125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="33.75" thickBot="1">
+    <row r="1" spans="1:14" ht="34.5" thickBot="1">
       <c r="A1" s="8" t="s">
         <v>15</v>
       </c>
@@ -2019,7 +2040,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="50.25" thickBot="1">
+    <row r="2" spans="1:14" ht="34.5" thickBot="1">
       <c r="A2" s="6">
         <v>100</v>
       </c>
@@ -2061,7 +2082,7 @@
       </c>
       <c r="N2" s="7"/>
     </row>
-    <row r="3" spans="1:14" ht="33.75" thickBot="1">
+    <row r="3" spans="1:14" ht="34.5" thickBot="1">
       <c r="A3" s="6">
         <v>101</v>
       </c>
@@ -2103,7 +2124,7 @@
       </c>
       <c r="N3" s="7"/>
     </row>
-    <row r="4" spans="1:14" ht="17.25" thickBot="1">
+    <row r="4" spans="1:14" ht="17.5" thickBot="1">
       <c r="A4" s="19">
         <v>102</v>
       </c>
@@ -2145,7 +2166,7 @@
       </c>
       <c r="N4" s="7"/>
     </row>
-    <row r="5" spans="1:14" ht="17.25" thickBot="1">
+    <row r="5" spans="1:14" ht="17.5" thickBot="1">
       <c r="A5" s="6">
         <v>103</v>
       </c>
@@ -2187,7 +2208,7 @@
       </c>
       <c r="N5" s="7"/>
     </row>
-    <row r="6" spans="1:14" ht="33.75" thickBot="1">
+    <row r="6" spans="1:14" ht="34.5" thickBot="1">
       <c r="A6" s="6">
         <v>131</v>
       </c>
@@ -2229,7 +2250,7 @@
       </c>
       <c r="N6" s="7"/>
     </row>
-    <row r="7" spans="1:14" ht="50.25" thickBot="1">
+    <row r="7" spans="1:14" ht="34.5" thickBot="1">
       <c r="A7" s="6">
         <v>200</v>
       </c>
@@ -2273,7 +2294,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="99.75" thickBot="1">
+    <row r="8" spans="1:14" ht="85.5" thickBot="1">
       <c r="A8" s="6">
         <v>201</v>
       </c>
@@ -2317,7 +2338,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="83.25" thickBot="1">
+    <row r="9" spans="1:14" ht="68.5" thickBot="1">
       <c r="A9" s="6">
         <v>202</v>
       </c>
@@ -2361,7 +2382,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="99.75" thickBot="1">
+    <row r="10" spans="1:14" ht="85.5" thickBot="1">
       <c r="A10" s="6">
         <v>203</v>
       </c>
@@ -2405,7 +2426,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="165.75" thickBot="1">
+    <row r="11" spans="1:14" ht="136.5" thickBot="1">
       <c r="A11" s="6">
         <v>231</v>
       </c>
@@ -2449,7 +2470,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="17.25" thickBot="1">
+    <row r="12" spans="1:14" ht="17.5" thickBot="1">
       <c r="A12" s="6">
         <v>232</v>
       </c>
@@ -2493,7 +2514,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="17.25" thickBot="1">
+    <row r="13" spans="1:14" ht="17.5" thickBot="1">
       <c r="A13" s="6">
         <v>300</v>
       </c>
@@ -2537,7 +2558,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="17.25" thickBot="1">
+    <row r="14" spans="1:14" ht="17.5" thickBot="1">
       <c r="A14" s="6">
         <v>301</v>
       </c>
@@ -2579,7 +2600,7 @@
       </c>
       <c r="N14" s="7"/>
     </row>
-    <row r="15" spans="1:14" ht="198.75" thickBot="1">
+    <row r="15" spans="1:14" ht="170.5" thickBot="1">
       <c r="A15" s="6">
         <v>302</v>
       </c>
@@ -2623,7 +2644,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="99.75" thickBot="1">
+    <row r="16" spans="1:14" ht="102.5" thickBot="1">
       <c r="A16" s="6">
         <v>303</v>
       </c>
@@ -2667,7 +2688,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="132.75" thickBot="1">
+    <row r="17" spans="1:14" ht="102.5" thickBot="1">
       <c r="A17" s="6">
         <v>331</v>
       </c>
@@ -2725,13 +2746,13 @@
       <selection activeCell="K29" sqref="K29:K48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="13.375" style="14" customWidth="1"/>
-    <col min="2" max="16384" width="8.625" style="14"/>
+    <col min="1" max="1" width="13.33203125" style="14" customWidth="1"/>
+    <col min="2" max="16384" width="8.58203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="49.5">
+    <row r="1" spans="1:16" ht="51">
       <c r="A1" s="26" t="s">
         <v>15</v>
       </c>
@@ -2831,7 +2852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="17.25" thickBot="1">
+    <row r="3" spans="1:16" ht="17.5" thickBot="1">
       <c r="A3" s="6">
         <v>100011102</v>
       </c>
@@ -2881,7 +2902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="33.75" thickBot="1">
+    <row r="4" spans="1:16" ht="34.5" thickBot="1">
       <c r="A4" s="6">
         <v>101012101</v>
       </c>
@@ -2931,7 +2952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="17.25" thickBot="1">
+    <row r="5" spans="1:16" ht="17.5" thickBot="1">
       <c r="A5" s="6">
         <v>101012102</v>
       </c>
@@ -2981,7 +3002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="33.75" thickBot="1">
+    <row r="6" spans="1:16" ht="34.5" thickBot="1">
       <c r="A6" s="6">
         <v>101012201</v>
       </c>
@@ -3031,7 +3052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="17.25" thickBot="1">
+    <row r="7" spans="1:16" ht="17.5" thickBot="1">
       <c r="A7" s="6">
         <v>101012202</v>
       </c>
@@ -3081,7 +3102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="33.75" thickBot="1">
+    <row r="8" spans="1:16" ht="34.5" thickBot="1">
       <c r="A8" s="6">
         <v>101012301</v>
       </c>
@@ -3131,7 +3152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="17.25" thickBot="1">
+    <row r="9" spans="1:16" ht="17.5" thickBot="1">
       <c r="A9" s="6">
         <v>101012302</v>
       </c>
@@ -3181,7 +3202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="33.75" thickBot="1">
+    <row r="10" spans="1:16" ht="34.5" thickBot="1">
       <c r="A10" s="6">
         <v>101012401</v>
       </c>
@@ -3231,7 +3252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="17.25" thickBot="1">
+    <row r="11" spans="1:16" ht="17.5" thickBot="1">
       <c r="A11" s="6">
         <v>101012402</v>
       </c>
@@ -3281,7 +3302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="33.75" thickBot="1">
+    <row r="12" spans="1:16" ht="34.5" thickBot="1">
       <c r="A12" s="6">
         <v>101012501</v>
       </c>
@@ -3331,7 +3352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="17.25" thickBot="1">
+    <row r="13" spans="1:16" ht="17.5" thickBot="1">
       <c r="A13" s="6">
         <v>101012502</v>
       </c>
@@ -3381,7 +3402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="17.25" thickBot="1">
+    <row r="14" spans="1:16" ht="17.5" thickBot="1">
       <c r="A14" s="32">
         <v>102012101</v>
       </c>
@@ -3431,7 +3452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="17.25" thickBot="1">
+    <row r="15" spans="1:16" ht="17.5" thickBot="1">
       <c r="A15" s="35">
         <v>102012102</v>
       </c>
@@ -3481,7 +3502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="17.25" thickBot="1">
+    <row r="16" spans="1:16" ht="17.5" thickBot="1">
       <c r="A16" s="35">
         <v>102012103</v>
       </c>
@@ -3531,7 +3552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="17.25" thickBot="1">
+    <row r="17" spans="1:16" ht="17.5" thickBot="1">
       <c r="A17" s="35">
         <v>102012201</v>
       </c>
@@ -3581,7 +3602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="17.25" thickBot="1">
+    <row r="18" spans="1:16" ht="17.5" thickBot="1">
       <c r="A18" s="35">
         <v>102012202</v>
       </c>
@@ -3631,7 +3652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="17.25" thickBot="1">
+    <row r="19" spans="1:16" ht="17.5" thickBot="1">
       <c r="A19" s="35">
         <v>102012203</v>
       </c>
@@ -3681,7 +3702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="17.25" thickBot="1">
+    <row r="20" spans="1:16" ht="17.5" thickBot="1">
       <c r="A20" s="35">
         <v>102012301</v>
       </c>
@@ -3731,7 +3752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="17.25" thickBot="1">
+    <row r="21" spans="1:16" ht="17.5" thickBot="1">
       <c r="A21" s="35">
         <v>102012302</v>
       </c>
@@ -3781,7 +3802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="17.25" thickBot="1">
+    <row r="22" spans="1:16" ht="17.5" thickBot="1">
       <c r="A22" s="35">
         <v>102012303</v>
       </c>
@@ -3831,7 +3852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="17.25" thickBot="1">
+    <row r="23" spans="1:16" ht="17.5" thickBot="1">
       <c r="A23" s="35">
         <v>102012401</v>
       </c>
@@ -3881,7 +3902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="17.25" thickBot="1">
+    <row r="24" spans="1:16" ht="17.5" thickBot="1">
       <c r="A24" s="35">
         <v>102012402</v>
       </c>
@@ -3931,7 +3952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="17.25" thickBot="1">
+    <row r="25" spans="1:16" ht="17.5" thickBot="1">
       <c r="A25" s="35">
         <v>102012403</v>
       </c>
@@ -3981,7 +4002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="17.25" thickBot="1">
+    <row r="26" spans="1:16" ht="17.5" thickBot="1">
       <c r="A26" s="35">
         <v>102012501</v>
       </c>
@@ -4031,7 +4052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="17.25" thickBot="1">
+    <row r="27" spans="1:16" ht="17.5" thickBot="1">
       <c r="A27" s="35">
         <v>102012502</v>
       </c>
@@ -4081,7 +4102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="17.25" thickBot="1">
+    <row r="28" spans="1:16" ht="17.5" thickBot="1">
       <c r="A28" s="38">
         <v>102012503</v>
       </c>
@@ -4131,7 +4152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="17.25" thickBot="1">
+    <row r="29" spans="1:16" ht="17.5" thickBot="1">
       <c r="A29" s="9">
         <v>103012101</v>
       </c>
@@ -4181,7 +4202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="50.25" thickBot="1">
+    <row r="30" spans="1:16" ht="34.5" thickBot="1">
       <c r="A30" s="9">
         <v>103012102</v>
       </c>
@@ -4231,7 +4252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="33.75" thickBot="1">
+    <row r="31" spans="1:16" ht="17.5" thickBot="1">
       <c r="A31" s="9">
         <v>103012103</v>
       </c>
@@ -4281,7 +4302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="33.75" thickBot="1">
+    <row r="32" spans="1:16" ht="17.5" thickBot="1">
       <c r="A32" s="9">
         <v>103012104</v>
       </c>
@@ -4331,7 +4352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="17.25" thickBot="1">
+    <row r="33" spans="1:16" ht="17.5" thickBot="1">
       <c r="A33" s="9">
         <v>103012201</v>
       </c>
@@ -4381,7 +4402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="50.25" thickBot="1">
+    <row r="34" spans="1:16" ht="34.5" thickBot="1">
       <c r="A34" s="9">
         <v>103012202</v>
       </c>
@@ -4431,7 +4452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="33.75" thickBot="1">
+    <row r="35" spans="1:16" ht="17.5" thickBot="1">
       <c r="A35" s="9">
         <v>103012203</v>
       </c>
@@ -4481,7 +4502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="33.75" thickBot="1">
+    <row r="36" spans="1:16" ht="17.5" thickBot="1">
       <c r="A36" s="9">
         <v>103012204</v>
       </c>
@@ -4531,7 +4552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="17.25" thickBot="1">
+    <row r="37" spans="1:16" ht="17.5" thickBot="1">
       <c r="A37" s="9">
         <v>103012301</v>
       </c>
@@ -4581,7 +4602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="50.25" thickBot="1">
+    <row r="38" spans="1:16" ht="34.5" thickBot="1">
       <c r="A38" s="9">
         <v>103012302</v>
       </c>
@@ -4631,7 +4652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="33.75" thickBot="1">
+    <row r="39" spans="1:16" ht="17.5" thickBot="1">
       <c r="A39" s="9">
         <v>103012303</v>
       </c>
@@ -4681,7 +4702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="33.75" thickBot="1">
+    <row r="40" spans="1:16" ht="17.5" thickBot="1">
       <c r="A40" s="9">
         <v>103012304</v>
       </c>
@@ -4731,7 +4752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="17.25" thickBot="1">
+    <row r="41" spans="1:16" ht="17.5" thickBot="1">
       <c r="A41" s="9">
         <v>103012401</v>
       </c>
@@ -4781,7 +4802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="50.25" thickBot="1">
+    <row r="42" spans="1:16" ht="34.5" thickBot="1">
       <c r="A42" s="9">
         <v>103012402</v>
       </c>
@@ -4831,7 +4852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="33.75" thickBot="1">
+    <row r="43" spans="1:16" ht="17.5" thickBot="1">
       <c r="A43" s="9">
         <v>103012403</v>
       </c>
@@ -4881,7 +4902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="33.75" thickBot="1">
+    <row r="44" spans="1:16" ht="17.5" thickBot="1">
       <c r="A44" s="9">
         <v>103012404</v>
       </c>
@@ -4931,7 +4952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="17.25" thickBot="1">
+    <row r="45" spans="1:16" ht="17.5" thickBot="1">
       <c r="A45" s="9">
         <v>103012501</v>
       </c>
@@ -4981,7 +5002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="50.25" thickBot="1">
+    <row r="46" spans="1:16" ht="34.5" thickBot="1">
       <c r="A46" s="9">
         <v>103012502</v>
       </c>
@@ -5031,7 +5052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="33.75" thickBot="1">
+    <row r="47" spans="1:16" ht="17.5" thickBot="1">
       <c r="A47" s="9">
         <v>103012503</v>
       </c>
@@ -5081,7 +5102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="33.75" thickBot="1">
+    <row r="48" spans="1:16" ht="17.5" thickBot="1">
       <c r="A48" s="9">
         <v>103012504</v>
       </c>
@@ -5131,7 +5152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:26" ht="17.25" thickBot="1">
+    <row r="49" spans="1:26" ht="17.5" thickBot="1">
       <c r="A49" s="6">
         <v>131013101</v>
       </c>
@@ -5191,7 +5212,7 @@
       <c r="Y49" s="7"/>
       <c r="Z49" s="7"/>
     </row>
-    <row r="50" spans="1:26" ht="17.25" thickBot="1">
+    <row r="50" spans="1:26" ht="17.5" thickBot="1">
       <c r="A50" s="6">
         <v>131013201</v>
       </c>
@@ -5251,7 +5272,7 @@
       <c r="Y50" s="7"/>
       <c r="Z50" s="7"/>
     </row>
-    <row r="51" spans="1:26" ht="17.25" thickBot="1">
+    <row r="51" spans="1:26" ht="17.5" thickBot="1">
       <c r="A51" s="6">
         <v>131013301</v>
       </c>
@@ -5311,7 +5332,7 @@
       <c r="Y51" s="7"/>
       <c r="Z51" s="7"/>
     </row>
-    <row r="52" spans="1:26" ht="17.25" thickBot="1">
+    <row r="52" spans="1:26" ht="17.5" thickBot="1">
       <c r="A52" s="6">
         <v>200021101</v>
       </c>
@@ -5361,7 +5382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:26" ht="17.25" thickBot="1">
+    <row r="53" spans="1:26" ht="17.5" thickBot="1">
       <c r="A53" s="6">
         <v>200021102</v>
       </c>
@@ -5411,7 +5432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:26" ht="17.25" thickBot="1">
+    <row r="54" spans="1:26" ht="17.5" thickBot="1">
       <c r="A54" s="6">
         <v>201022101</v>
       </c>
@@ -5461,7 +5482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:26" ht="17.25" thickBot="1">
+    <row r="55" spans="1:26" ht="17.5" thickBot="1">
       <c r="A55" s="6">
         <v>201022102</v>
       </c>
@@ -5511,7 +5532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:26" ht="17.25" thickBot="1">
+    <row r="56" spans="1:26" ht="17.5" thickBot="1">
       <c r="A56" s="6">
         <v>201022201</v>
       </c>
@@ -5561,7 +5582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:26" ht="17.25" thickBot="1">
+    <row r="57" spans="1:26" ht="17.5" thickBot="1">
       <c r="A57" s="6">
         <v>201022202</v>
       </c>
@@ -5611,7 +5632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:26" ht="17.25" thickBot="1">
+    <row r="58" spans="1:26" ht="17.5" thickBot="1">
       <c r="A58" s="6">
         <v>201022301</v>
       </c>
@@ -5661,7 +5682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:26" ht="17.25" thickBot="1">
+    <row r="59" spans="1:26" ht="17.5" thickBot="1">
       <c r="A59" s="6">
         <v>201022302</v>
       </c>
@@ -5711,7 +5732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:26" ht="17.25" thickBot="1">
+    <row r="60" spans="1:26" ht="17.5" thickBot="1">
       <c r="A60" s="6">
         <v>201022401</v>
       </c>
@@ -5761,7 +5782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:26" ht="17.25" thickBot="1">
+    <row r="61" spans="1:26" ht="17.5" thickBot="1">
       <c r="A61" s="6">
         <v>201022402</v>
       </c>
@@ -5811,7 +5832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:26" ht="17.25" thickBot="1">
+    <row r="62" spans="1:26" ht="17.5" thickBot="1">
       <c r="A62" s="6">
         <v>201022501</v>
       </c>
@@ -5861,7 +5882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:26" ht="17.25" thickBot="1">
+    <row r="63" spans="1:26" ht="17.5" thickBot="1">
       <c r="A63" s="6">
         <v>201022502</v>
       </c>
@@ -5911,7 +5932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:26" ht="17.25" thickBot="1">
+    <row r="64" spans="1:26" ht="17.5" thickBot="1">
       <c r="A64" s="6">
         <v>201022111</v>
       </c>
@@ -5961,7 +5982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:16" ht="33.75" thickBot="1">
+    <row r="65" spans="1:16" ht="34.5" thickBot="1">
       <c r="A65" s="6">
         <v>201022112</v>
       </c>
@@ -6011,7 +6032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:16" ht="17.25" thickBot="1">
+    <row r="66" spans="1:16" ht="17.5" thickBot="1">
       <c r="A66" s="6">
         <v>201022211</v>
       </c>
@@ -6061,7 +6082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:16" ht="33.75" thickBot="1">
+    <row r="67" spans="1:16" ht="34.5" thickBot="1">
       <c r="A67" s="6">
         <v>201022212</v>
       </c>
@@ -6111,7 +6132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:16" ht="17.25" thickBot="1">
+    <row r="68" spans="1:16" ht="17.5" thickBot="1">
       <c r="A68" s="6">
         <v>201022311</v>
       </c>
@@ -6161,7 +6182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:16" ht="33.75" thickBot="1">
+    <row r="69" spans="1:16" ht="34.5" thickBot="1">
       <c r="A69" s="6">
         <v>201022312</v>
       </c>
@@ -6211,7 +6232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:16" ht="17.25" thickBot="1">
+    <row r="70" spans="1:16" ht="17.5" thickBot="1">
       <c r="A70" s="6">
         <v>201022411</v>
       </c>
@@ -6261,7 +6282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:16" ht="33.75" thickBot="1">
+    <row r="71" spans="1:16" ht="34.5" thickBot="1">
       <c r="A71" s="6">
         <v>201022412</v>
       </c>
@@ -6311,7 +6332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:16" ht="17.25" thickBot="1">
+    <row r="72" spans="1:16" ht="17.5" thickBot="1">
       <c r="A72" s="6">
         <v>201022511</v>
       </c>
@@ -6361,7 +6382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:16" ht="33.75" thickBot="1">
+    <row r="73" spans="1:16" ht="34.5" thickBot="1">
       <c r="A73" s="6">
         <v>201022512</v>
       </c>
@@ -6411,7 +6432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:16" ht="17.25" thickBot="1">
+    <row r="74" spans="1:16" ht="17.5" thickBot="1">
       <c r="A74" s="6">
         <v>201022121</v>
       </c>
@@ -6461,7 +6482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:16" ht="33.75" thickBot="1">
+    <row r="75" spans="1:16" ht="34.5" thickBot="1">
       <c r="A75" s="6">
         <v>201022122</v>
       </c>
@@ -6511,7 +6532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:16" ht="33.75" thickBot="1">
+    <row r="76" spans="1:16" ht="34.5" thickBot="1">
       <c r="A76" s="6">
         <v>201022123</v>
       </c>
@@ -6561,7 +6582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:16" ht="17.25" thickBot="1">
+    <row r="77" spans="1:16" ht="17.5" thickBot="1">
       <c r="A77" s="6">
         <v>201022221</v>
       </c>
@@ -6611,7 +6632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:16" ht="33.75" thickBot="1">
+    <row r="78" spans="1:16" ht="34.5" thickBot="1">
       <c r="A78" s="6">
         <v>201022222</v>
       </c>
@@ -6661,7 +6682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:16" ht="33.75" thickBot="1">
+    <row r="79" spans="1:16" ht="34.5" thickBot="1">
       <c r="A79" s="6">
         <v>201022223</v>
       </c>
@@ -6711,7 +6732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:16" ht="17.25" thickBot="1">
+    <row r="80" spans="1:16" ht="17.5" thickBot="1">
       <c r="A80" s="6">
         <v>201022321</v>
       </c>
@@ -6761,7 +6782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:16" ht="33.75" thickBot="1">
+    <row r="81" spans="1:16" ht="34.5" thickBot="1">
       <c r="A81" s="6">
         <v>201022322</v>
       </c>
@@ -6811,7 +6832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:16" ht="33.75" thickBot="1">
+    <row r="82" spans="1:16" ht="34.5" thickBot="1">
       <c r="A82" s="6">
         <v>201022323</v>
       </c>
@@ -6861,7 +6882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:16" ht="17.25" thickBot="1">
+    <row r="83" spans="1:16" ht="17.5" thickBot="1">
       <c r="A83" s="6">
         <v>201022421</v>
       </c>
@@ -6911,7 +6932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:16" ht="33.75" thickBot="1">
+    <row r="84" spans="1:16" ht="34.5" thickBot="1">
       <c r="A84" s="6">
         <v>201022422</v>
       </c>
@@ -6961,7 +6982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:16" ht="33.75" thickBot="1">
+    <row r="85" spans="1:16" ht="34.5" thickBot="1">
       <c r="A85" s="6">
         <v>201022423</v>
       </c>
@@ -7011,7 +7032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:16" ht="17.25" thickBot="1">
+    <row r="86" spans="1:16" ht="17.5" thickBot="1">
       <c r="A86" s="6">
         <v>201022521</v>
       </c>
@@ -7061,7 +7082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:16" ht="33.75" thickBot="1">
+    <row r="87" spans="1:16" ht="34.5" thickBot="1">
       <c r="A87" s="6">
         <v>201022522</v>
       </c>
@@ -7111,7 +7132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:16" ht="33.75" thickBot="1">
+    <row r="88" spans="1:16" ht="34.5" thickBot="1">
       <c r="A88" s="6">
         <v>201022523</v>
       </c>
@@ -7161,7 +7182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:16" ht="17.25" thickBot="1">
+    <row r="89" spans="1:16" ht="17.5" thickBot="1">
       <c r="A89" s="6">
         <v>202022101</v>
       </c>
@@ -7211,7 +7232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:16" ht="17.25" thickBot="1">
+    <row r="90" spans="1:16" ht="17.5" thickBot="1">
       <c r="A90" s="6">
         <v>202022201</v>
       </c>
@@ -7261,7 +7282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:16" ht="17.25" thickBot="1">
+    <row r="91" spans="1:16" ht="17.5" thickBot="1">
       <c r="A91" s="6">
         <v>202022301</v>
       </c>
@@ -7311,7 +7332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:16" ht="17.25" thickBot="1">
+    <row r="92" spans="1:16" ht="17.5" thickBot="1">
       <c r="A92" s="6">
         <v>202022401</v>
       </c>
@@ -7361,7 +7382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:16" ht="17.25" thickBot="1">
+    <row r="93" spans="1:16" ht="17.5" thickBot="1">
       <c r="A93" s="6">
         <v>202022501</v>
       </c>
@@ -7411,7 +7432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:16" ht="17.25" thickBot="1">
+    <row r="94" spans="1:16" ht="17.5" thickBot="1">
       <c r="A94" s="6">
         <v>203022101</v>
       </c>
@@ -7461,7 +7482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:16" ht="17.25" thickBot="1">
+    <row r="95" spans="1:16" ht="17.5" thickBot="1">
       <c r="A95" s="6">
         <v>203022102</v>
       </c>
@@ -7511,7 +7532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:16" ht="17.25" thickBot="1">
+    <row r="96" spans="1:16" ht="17.5" thickBot="1">
       <c r="A96" s="6">
         <v>203022103</v>
       </c>
@@ -7561,7 +7582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:16" ht="17.25" thickBot="1">
+    <row r="97" spans="1:16" ht="17.5" thickBot="1">
       <c r="A97" s="6">
         <v>203022201</v>
       </c>
@@ -7611,7 +7632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:16" ht="17.25" thickBot="1">
+    <row r="98" spans="1:16" ht="17.5" thickBot="1">
       <c r="A98" s="6">
         <v>203022202</v>
       </c>
@@ -7661,7 +7682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:16" ht="17.25" thickBot="1">
+    <row r="99" spans="1:16" ht="17.5" thickBot="1">
       <c r="A99" s="6">
         <v>203022203</v>
       </c>
@@ -7711,7 +7732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:16" ht="17.25" thickBot="1">
+    <row r="100" spans="1:16" ht="17.5" thickBot="1">
       <c r="A100" s="6">
         <v>203022301</v>
       </c>
@@ -7761,7 +7782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:16" ht="17.25" thickBot="1">
+    <row r="101" spans="1:16" ht="17.5" thickBot="1">
       <c r="A101" s="6">
         <v>203022302</v>
       </c>
@@ -7811,7 +7832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:16" ht="17.25" thickBot="1">
+    <row r="102" spans="1:16" ht="17.5" thickBot="1">
       <c r="A102" s="6">
         <v>203022303</v>
       </c>
@@ -7861,7 +7882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:16" ht="17.25" thickBot="1">
+    <row r="103" spans="1:16" ht="17.5" thickBot="1">
       <c r="A103" s="6">
         <v>203022401</v>
       </c>
@@ -7911,7 +7932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:16" ht="17.25" thickBot="1">
+    <row r="104" spans="1:16" ht="17.5" thickBot="1">
       <c r="A104" s="6">
         <v>203022402</v>
       </c>
@@ -7961,7 +7982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:16" ht="17.25" thickBot="1">
+    <row r="105" spans="1:16" ht="17.5" thickBot="1">
       <c r="A105" s="6">
         <v>203022403</v>
       </c>
@@ -8011,7 +8032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:16" ht="17.25" thickBot="1">
+    <row r="106" spans="1:16" ht="17.5" thickBot="1">
       <c r="A106" s="6">
         <v>203022501</v>
       </c>
@@ -8061,7 +8082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:16" ht="17.25" thickBot="1">
+    <row r="107" spans="1:16" ht="17.5" thickBot="1">
       <c r="A107" s="6">
         <v>203022502</v>
       </c>
@@ -8111,7 +8132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:16" ht="17.25" thickBot="1">
+    <row r="108" spans="1:16" ht="17.5" thickBot="1">
       <c r="A108" s="6">
         <v>203022503</v>
       </c>
@@ -8161,7 +8182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:16" ht="50.25" thickBot="1">
+    <row r="109" spans="1:16" ht="34.5" thickBot="1">
       <c r="A109" s="6">
         <v>231023101</v>
       </c>
@@ -8211,7 +8232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:16" ht="50.25" thickBot="1">
+    <row r="110" spans="1:16" ht="34.5" thickBot="1">
       <c r="A110" s="6">
         <v>231023201</v>
       </c>
@@ -8261,7 +8282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:16" ht="50.25" thickBot="1">
+    <row r="111" spans="1:16" ht="34.5" thickBot="1">
       <c r="A111" s="6">
         <v>231023301</v>
       </c>
@@ -8311,7 +8332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:16" ht="17.25" thickBot="1">
+    <row r="112" spans="1:16" ht="17.5" thickBot="1">
       <c r="A112" s="6">
         <v>232023101</v>
       </c>
@@ -8361,7 +8382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:16" ht="17.25" thickBot="1">
+    <row r="113" spans="1:16" ht="17.5" thickBot="1">
       <c r="A113" s="6">
         <v>232023102</v>
       </c>
@@ -8411,7 +8432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:16" ht="17.25" thickBot="1">
+    <row r="114" spans="1:16" ht="17.5" thickBot="1">
       <c r="A114" s="6">
         <v>232023201</v>
       </c>
@@ -8461,7 +8482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:16" ht="17.25" thickBot="1">
+    <row r="115" spans="1:16" ht="17.5" thickBot="1">
       <c r="A115" s="6">
         <v>232023202</v>
       </c>
@@ -8511,7 +8532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:16" ht="17.25" thickBot="1">
+    <row r="116" spans="1:16" ht="17.5" thickBot="1">
       <c r="A116" s="6">
         <v>232023301</v>
       </c>
@@ -8561,7 +8582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:16" ht="17.25" thickBot="1">
+    <row r="117" spans="1:16" ht="17.5" thickBot="1">
       <c r="A117" s="6">
         <v>232023302</v>
       </c>
@@ -8611,7 +8632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:16" ht="17.25" thickBot="1">
+    <row r="118" spans="1:16" ht="17.5" thickBot="1">
       <c r="A118" s="1">
         <v>300031101</v>
       </c>
@@ -8661,7 +8682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:16" ht="45.75" thickBot="1">
+    <row r="119" spans="1:16" ht="44" thickBot="1">
       <c r="A119" s="1">
         <v>301032101</v>
       </c>
@@ -8711,7 +8732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:16" ht="45.75" thickBot="1">
+    <row r="120" spans="1:16" ht="44" thickBot="1">
       <c r="A120" s="1">
         <v>301032201</v>
       </c>
@@ -8761,7 +8782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:16" ht="45.75" thickBot="1">
+    <row r="121" spans="1:16" ht="44" thickBot="1">
       <c r="A121" s="1">
         <v>301032301</v>
       </c>
@@ -8811,7 +8832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:16" ht="45.75" thickBot="1">
+    <row r="122" spans="1:16" ht="44" thickBot="1">
       <c r="A122" s="1">
         <v>301032401</v>
       </c>
@@ -8861,7 +8882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:16" ht="45.75" thickBot="1">
+    <row r="123" spans="1:16" ht="44" thickBot="1">
       <c r="A123" s="1">
         <v>301032501</v>
       </c>
@@ -8911,7 +8932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:16" ht="17.25" thickBot="1">
+    <row r="124" spans="1:16" ht="17.5" thickBot="1">
       <c r="A124" s="1">
         <v>302032101</v>
       </c>
@@ -8961,7 +8982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:16" ht="17.25" thickBot="1">
+    <row r="125" spans="1:16" ht="17.5" thickBot="1">
       <c r="A125" s="1">
         <v>302032201</v>
       </c>
@@ -9011,7 +9032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:16" ht="17.25" thickBot="1">
+    <row r="126" spans="1:16" ht="17.5" thickBot="1">
       <c r="A126" s="1">
         <v>302032301</v>
       </c>
@@ -9061,7 +9082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:16" ht="17.25" thickBot="1">
+    <row r="127" spans="1:16" ht="17.5" thickBot="1">
       <c r="A127" s="1">
         <v>302032401</v>
       </c>
@@ -9111,7 +9132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:16" ht="17.25" thickBot="1">
+    <row r="128" spans="1:16" ht="17.5" thickBot="1">
       <c r="A128" s="1">
         <v>302032501</v>
       </c>
@@ -9161,7 +9182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:16" ht="17.25" thickBot="1">
+    <row r="129" spans="1:16" ht="17.5" thickBot="1">
       <c r="A129" s="1">
         <v>303032101</v>
       </c>
@@ -9211,7 +9232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:16" ht="17.25" thickBot="1">
+    <row r="130" spans="1:16" ht="17.5" thickBot="1">
       <c r="A130" s="1">
         <v>303032102</v>
       </c>
@@ -9261,7 +9282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:16" ht="17.25" thickBot="1">
+    <row r="131" spans="1:16" ht="17.5" thickBot="1">
       <c r="A131" s="1">
         <v>303032201</v>
       </c>
@@ -9311,7 +9332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:16" ht="17.25" thickBot="1">
+    <row r="132" spans="1:16" ht="17.5" thickBot="1">
       <c r="A132" s="1">
         <v>303032202</v>
       </c>
@@ -9361,7 +9382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:16" ht="17.25" thickBot="1">
+    <row r="133" spans="1:16" ht="17.5" thickBot="1">
       <c r="A133" s="1">
         <v>303032301</v>
       </c>
@@ -9411,7 +9432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:16" ht="17.25" thickBot="1">
+    <row r="134" spans="1:16" ht="17.5" thickBot="1">
       <c r="A134" s="1">
         <v>303032302</v>
       </c>
@@ -9461,7 +9482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:16" ht="17.25" thickBot="1">
+    <row r="135" spans="1:16" ht="17.5" thickBot="1">
       <c r="A135" s="1">
         <v>303032401</v>
       </c>
@@ -9511,7 +9532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:16" ht="17.25" thickBot="1">
+    <row r="136" spans="1:16" ht="17.5" thickBot="1">
       <c r="A136" s="1">
         <v>303032402</v>
       </c>
@@ -9561,7 +9582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:16" ht="17.25" thickBot="1">
+    <row r="137" spans="1:16" ht="17.5" thickBot="1">
       <c r="A137" s="1">
         <v>303032501</v>
       </c>
@@ -9611,7 +9632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:16" ht="17.25" thickBot="1">
+    <row r="138" spans="1:16" ht="17.5" thickBot="1">
       <c r="A138" s="1">
         <v>303032502</v>
       </c>
@@ -9661,7 +9682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:16" ht="17.25" thickBot="1">
+    <row r="139" spans="1:16" ht="17.5" thickBot="1">
       <c r="A139" s="1">
         <v>331033101</v>
       </c>
@@ -9711,7 +9732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:16" ht="17.25" thickBot="1">
+    <row r="140" spans="1:16" ht="17.5" thickBot="1">
       <c r="A140" s="1">
         <v>331033201</v>
       </c>
@@ -9761,7 +9782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:16" ht="17.25" thickBot="1">
+    <row r="141" spans="1:16" ht="17.5" thickBot="1">
       <c r="A141" s="1">
         <v>331033301</v>
       </c>
@@ -9826,12 +9847,12 @@
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="16384" width="8.625" style="14"/>
+    <col min="1" max="16384" width="8.58203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.25" thickBot="1">
+    <row r="1" spans="1:7" ht="17.5" thickBot="1">
       <c r="A1" s="8" t="s">
         <v>15</v>
       </c>
@@ -9851,7 +9872,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="17.25" thickBot="1">
+    <row r="2" spans="1:7" ht="17.5" thickBot="1">
       <c r="A2" s="6">
         <v>100</v>
       </c>
@@ -9891,7 +9912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="17.25" thickBot="1">
+    <row r="4" spans="1:7" ht="17.5" thickBot="1">
       <c r="A4" s="19">
         <v>102</v>
       </c>
@@ -9911,7 +9932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="17.25" thickBot="1">
+    <row r="5" spans="1:7" ht="17.5" thickBot="1">
       <c r="A5" s="6">
         <v>103</v>
       </c>
@@ -9931,7 +9952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="17.25" thickBot="1">
+    <row r="6" spans="1:7" ht="17.5" thickBot="1">
       <c r="A6" s="6">
         <v>131</v>
       </c>
@@ -9951,7 +9972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="17.25" thickBot="1">
+    <row r="7" spans="1:7" ht="17.5" thickBot="1">
       <c r="A7" s="6">
         <v>200</v>
       </c>
@@ -9972,7 +9993,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:7" ht="17.25" thickBot="1">
+    <row r="8" spans="1:7" ht="17.5" thickBot="1">
       <c r="A8" s="6">
         <v>201</v>
       </c>
@@ -9992,7 +10013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="17.25" thickBot="1">
+    <row r="9" spans="1:7" ht="17.5" thickBot="1">
       <c r="A9" s="6">
         <v>202</v>
       </c>
@@ -10012,7 +10033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="17.25" thickBot="1">
+    <row r="10" spans="1:7" ht="17.5" thickBot="1">
       <c r="A10" s="6">
         <v>203</v>
       </c>
@@ -10032,7 +10053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="17.25" thickBot="1">
+    <row r="11" spans="1:7" ht="17.5" thickBot="1">
       <c r="A11" s="6">
         <v>231</v>
       </c>
@@ -10052,7 +10073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="17.25" thickBot="1">
+    <row r="12" spans="1:7" ht="17.5" thickBot="1">
       <c r="A12" s="6">
         <v>232</v>
       </c>
@@ -10072,7 +10093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="17.25" thickBot="1">
+    <row r="13" spans="1:7" ht="17.5" thickBot="1">
       <c r="A13" s="6">
         <v>300</v>
       </c>
@@ -10092,7 +10113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="17.25" thickBot="1">
+    <row r="14" spans="1:7" ht="17.5" thickBot="1">
       <c r="A14" s="6">
         <v>301</v>
       </c>
@@ -10112,7 +10133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="17.25" thickBot="1">
+    <row r="15" spans="1:7" ht="17.5" thickBot="1">
       <c r="A15" s="6">
         <v>302</v>
       </c>
@@ -10132,7 +10153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="17.25" thickBot="1">
+    <row r="16" spans="1:7" ht="17.5" thickBot="1">
       <c r="A16" s="6">
         <v>303</v>
       </c>
@@ -10152,7 +10173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="17.25" thickBot="1">
+    <row r="17" spans="1:6" ht="17.5" thickBot="1">
       <c r="A17" s="6">
         <v>331</v>
       </c>
@@ -10187,19 +10208,19 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="8.625" style="14"/>
+    <col min="1" max="1" width="8.58203125" style="14"/>
     <col min="2" max="2" width="14" style="14" customWidth="1"/>
     <col min="3" max="3" width="11.25" style="14" customWidth="1"/>
-    <col min="4" max="8" width="8.625" style="14"/>
-    <col min="9" max="9" width="13.375" style="14" customWidth="1"/>
-    <col min="10" max="10" width="8.625" style="14" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="9.375" style="14" customWidth="1"/>
-    <col min="12" max="16384" width="8.625" style="14"/>
+    <col min="4" max="8" width="8.58203125" style="14"/>
+    <col min="9" max="9" width="13.33203125" style="14" customWidth="1"/>
+    <col min="10" max="10" width="8.58203125" style="14" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="9.33203125" style="14" customWidth="1"/>
+    <col min="12" max="16384" width="8.58203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="33.75" thickBot="1">
+    <row r="1" spans="1:16" ht="34.5" thickBot="1">
       <c r="A1" s="10" t="s">
         <v>15</v>
       </c>
@@ -10249,7 +10270,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="17.25" thickBot="1">
+    <row r="2" spans="1:16" ht="17.5" thickBot="1">
       <c r="A2" s="6">
         <v>1000</v>
       </c>
@@ -10299,7 +10320,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="17.25" thickBot="1">
+    <row r="3" spans="1:16" ht="17.5" thickBot="1">
       <c r="A3" s="6">
         <v>2000</v>
       </c>
@@ -10349,7 +10370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="17.25" thickBot="1">
+    <row r="4" spans="1:16" ht="17.5" thickBot="1">
       <c r="A4" s="6">
         <v>3000</v>
       </c>
@@ -10413,7 +10434,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
@@ -10511,18 +10532,18 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B4BE54-90AE-4DAF-BA80-4CA3867A9D82}">
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:T4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="16384" width="8.625" style="14"/>
+    <col min="1" max="16384" width="8.58203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="33.75" thickBot="1">
+    <row r="1" spans="1:21" ht="34.5" thickBot="1">
       <c r="A1" s="46" t="s">
         <v>15</v>
       </c>
@@ -10583,9 +10604,11 @@
       <c r="T1" s="62" t="s">
         <v>160</v>
       </c>
-      <c r="U1" s="7"/>
-    </row>
-    <row r="2" spans="1:21" ht="30.75" thickBot="1">
+      <c r="U1" s="65" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="29.5" thickBot="1">
       <c r="A2" s="1">
         <v>1000</v>
       </c>
@@ -10593,26 +10616,26 @@
         <v>112</v>
       </c>
       <c r="C2" s="1">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="D2" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="E2" s="1">
+      <c r="G2" s="1">
         <v>150</v>
       </c>
-      <c r="F2" s="1">
+      <c r="H2" s="1">
         <v>5</v>
       </c>
-      <c r="G2" s="1">
+      <c r="I2" s="1">
         <v>5</v>
       </c>
-      <c r="H2" s="1">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1">
-        <v>0</v>
-      </c>
       <c r="J2" s="1">
         <v>0</v>
       </c>
@@ -10623,14 +10646,14 @@
         <v>0</v>
       </c>
       <c r="M2" s="1">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1">
         <v>0.1</v>
       </c>
-      <c r="N2" s="1">
-        <v>0</v>
-      </c>
-      <c r="O2" s="1">
-        <v>0</v>
-      </c>
       <c r="P2" s="1">
         <v>0</v>
       </c>
@@ -10646,9 +10669,11 @@
       <c r="T2" s="1">
         <v>0</v>
       </c>
-      <c r="U2" s="7"/>
-    </row>
-    <row r="3" spans="1:21" ht="30.75" thickBot="1">
+      <c r="U2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="29.5" thickBot="1">
       <c r="A3" s="1">
         <v>2000</v>
       </c>
@@ -10656,119 +10681,243 @@
         <v>114</v>
       </c>
       <c r="C3" s="1">
+        <v>1001</v>
+      </c>
+      <c r="D3" s="44" t="s">
+        <v>188</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="44" t="s">
+        <v>113</v>
+      </c>
+      <c r="G3" s="1">
+        <v>200</v>
+      </c>
+      <c r="H3" s="1">
+        <v>5</v>
+      </c>
+      <c r="I3" s="1">
+        <v>7</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="P3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>0</v>
+      </c>
+      <c r="R3" s="1">
+        <v>0</v>
+      </c>
+      <c r="S3" s="1">
+        <v>0</v>
+      </c>
+      <c r="T3" s="1">
+        <v>0</v>
+      </c>
+      <c r="U3" s="1">
         <v>2</v>
       </c>
-      <c r="D3" s="44" t="s">
-        <v>115</v>
-      </c>
-      <c r="E3" s="1">
-        <v>700</v>
-      </c>
-      <c r="F3" s="1">
-        <v>5</v>
-      </c>
-      <c r="G3" s="1">
-        <v>10</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1">
-        <v>0</v>
-      </c>
-      <c r="K3" s="1">
-        <v>0</v>
-      </c>
-      <c r="L3" s="1">
-        <v>0</v>
-      </c>
-      <c r="M3" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="N3" s="1">
-        <v>0</v>
-      </c>
-      <c r="O3" s="1">
-        <v>0</v>
-      </c>
-      <c r="P3" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>0</v>
-      </c>
-      <c r="R3" s="1">
-        <v>0</v>
-      </c>
-      <c r="S3" s="1">
-        <v>0</v>
-      </c>
-      <c r="T3" s="1">
-        <v>0</v>
-      </c>
-      <c r="U3" s="7"/>
-    </row>
-    <row r="4" spans="1:21" ht="17.25" thickBot="1">
+    </row>
+    <row r="4" spans="1:21" ht="29.5" thickBot="1">
       <c r="A4" s="7">
         <v>3000</v>
       </c>
       <c r="B4" s="7"/>
-      <c r="C4" s="7">
+      <c r="C4" s="1">
+        <v>1002</v>
+      </c>
+      <c r="D4" s="44" t="s">
+        <v>189</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="44" t="s">
+        <v>113</v>
+      </c>
+      <c r="G4" s="1">
+        <v>250</v>
+      </c>
+      <c r="H4" s="1">
+        <v>5</v>
+      </c>
+      <c r="I4" s="1">
+        <v>10</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>0</v>
+      </c>
+      <c r="R4" s="1">
+        <v>0</v>
+      </c>
+      <c r="S4" s="1">
+        <v>0</v>
+      </c>
+      <c r="T4" s="1">
+        <v>0</v>
+      </c>
+      <c r="U4" s="1">
         <v>3</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="1">
+    </row>
+    <row r="5" spans="1:21" ht="29.5" thickBot="1">
+      <c r="C5" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D5" s="44" t="s">
+        <v>114</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2</v>
+      </c>
+      <c r="F5" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="G5" s="1">
         <v>700</v>
       </c>
-      <c r="F4" s="1">
+      <c r="H5" s="1">
         <v>5</v>
       </c>
-      <c r="G4" s="1">
-        <v>10</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0</v>
-      </c>
-      <c r="J4" s="1">
-        <v>0</v>
-      </c>
-      <c r="K4" s="1">
-        <v>0</v>
-      </c>
-      <c r="L4" s="1">
-        <v>0</v>
-      </c>
-      <c r="M4" s="1">
+      <c r="I5" s="1">
+        <v>20</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
         <v>0.2</v>
       </c>
-      <c r="N4" s="1">
-        <v>0</v>
-      </c>
-      <c r="O4" s="1">
-        <v>0</v>
-      </c>
-      <c r="P4" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>0</v>
-      </c>
-      <c r="R4" s="1">
-        <v>0</v>
-      </c>
-      <c r="S4" s="1">
-        <v>0</v>
-      </c>
-      <c r="T4" s="1">
-        <v>0</v>
-      </c>
-      <c r="U4" s="7"/>
+      <c r="P5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>0</v>
+      </c>
+      <c r="R5" s="1">
+        <v>0</v>
+      </c>
+      <c r="S5" s="1">
+        <v>0</v>
+      </c>
+      <c r="T5" s="1">
+        <v>0</v>
+      </c>
+      <c r="U5" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="29.5" thickBot="1">
+      <c r="C6" s="1">
+        <v>2001</v>
+      </c>
+      <c r="D6" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2</v>
+      </c>
+      <c r="F6" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="G6" s="1">
+        <v>800</v>
+      </c>
+      <c r="H6" s="1">
+        <v>5</v>
+      </c>
+      <c r="I6" s="1">
+        <v>30</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0</v>
+      </c>
+      <c r="M6" s="1">
+        <v>0</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="P6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>0</v>
+      </c>
+      <c r="R6" s="1">
+        <v>0</v>
+      </c>
+      <c r="S6" s="1">
+        <v>0</v>
+      </c>
+      <c r="T6" s="1">
+        <v>0</v>
+      </c>
+      <c r="U6" s="1">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -10785,12 +10934,12 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
-    <col min="10" max="10" width="18.375" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="33.75" thickBot="1">
+    <row r="1" spans="1:10" ht="34.5" thickBot="1">
       <c r="A1" s="52" t="s">
         <v>15</v>
       </c>
@@ -10822,7 +10971,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17.25" thickBot="1">
+    <row r="2" spans="1:10" ht="17.5" thickBot="1">
       <c r="A2" s="9">
         <v>100000</v>
       </c>
@@ -10854,7 +11003,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="17.25" thickBot="1">
+    <row r="3" spans="1:10" ht="17.5" thickBot="1">
       <c r="A3" s="9">
         <v>200000</v>
       </c>
@@ -10900,16 +11049,16 @@
       <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
-    <col min="2" max="2" width="12.875" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
     <col min="9" max="9" width="12.25" customWidth="1"/>
-    <col min="11" max="11" width="12.625" customWidth="1"/>
-    <col min="12" max="12" width="15.125" customWidth="1"/>
-    <col min="13" max="13" width="18.125" customWidth="1"/>
+    <col min="11" max="11" width="12.58203125" customWidth="1"/>
+    <col min="12" max="12" width="15.08203125" customWidth="1"/>
+    <col min="13" max="13" width="18.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="33.75" thickBot="1">
+    <row r="1" spans="1:14" ht="34.5" thickBot="1">
       <c r="A1" s="58" t="s">
         <v>15</v>
       </c>
@@ -10951,7 +11100,7 @@
       </c>
       <c r="N1" s="18"/>
     </row>
-    <row r="2" spans="1:14" ht="17.25" thickBot="1">
+    <row r="2" spans="1:14" ht="17.5" thickBot="1">
       <c r="A2" s="9">
         <v>1000001</v>
       </c>
@@ -10993,7 +11142,7 @@
       </c>
       <c r="N2" s="18"/>
     </row>
-    <row r="3" spans="1:14" ht="17.25" thickBot="1">
+    <row r="3" spans="1:14" ht="17.5" thickBot="1">
       <c r="A3" s="9">
         <v>2000001</v>
       </c>

</xml_diff>

<commit_message>
level up error fix
</commit_message>
<xml_diff>
--- a/Assets/04Table/TS.xlsx
+++ b/Assets/04Table/TS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cksgm\Unity\ProjectTS\Assets\04Table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77CC8095-CC61-4FA1-A77E-52C7538BDFD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C581AD8-6C77-4948-B4FF-4A92FF30EAB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="400" windowWidth="18800" windowHeight="13280" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Player_Stats" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="243">
   <si>
     <t>Level</t>
   </si>
@@ -135,13 +135,7 @@
     <t>CS_Basic</t>
   </si>
   <si>
-    <t>트와이스 커터</t>
-  </si>
-  <si>
     <t>Twice_Cutter</t>
-  </si>
-  <si>
-    <t>라이징 슬래쉬</t>
   </si>
   <si>
     <t>Rising_Slash</t>
@@ -151,37 +145,19 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>부스트 해머 일반 공격</t>
-  </si>
-  <si>
     <t>BH_Basic</t>
   </si>
   <si>
-    <t>고르디우스의 바퀴</t>
-  </si>
-  <si>
     <t>Gordian_Wheel</t>
   </si>
   <si>
-    <t>승룡추</t>
-  </si>
-  <si>
     <t>Dragon_Hammer</t>
   </si>
   <si>
-    <t>인력장</t>
-  </si>
-  <si>
     <t>Attraction_Field</t>
   </si>
   <si>
-    <t>윤회</t>
-  </si>
-  <si>
     <t>Samsara</t>
-  </si>
-  <si>
-    <t>나락</t>
   </si>
   <si>
     <t>Naraka</t>
@@ -191,31 +167,16 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>플라즈마 라이플 일반 공격</t>
-  </si>
-  <si>
     <t>PR_Basic</t>
   </si>
   <si>
-    <t>PG - 15</t>
-  </si>
-  <si>
     <t>PG_15</t>
   </si>
   <si>
-    <t>철갑 사격</t>
-  </si>
-  <si>
     <t>APHE_Shoot</t>
   </si>
   <si>
-    <t>핀 포인트 다운</t>
-  </si>
-  <si>
     <t>Pin_Point_Down</t>
-  </si>
-  <si>
-    <t>지정 섬멸</t>
   </si>
   <si>
     <t>Designated_Eliminate</t>
@@ -421,9 +382,6 @@
     <t>정예 크리처</t>
   </si>
   <si>
-    <t>어니스트</t>
-  </si>
-  <si>
     <t>Honest</t>
   </si>
   <si>
@@ -440,9 +398,6 @@
     <t>Linked_Skill</t>
   </si>
   <si>
-    <t>디멘션 디스토션</t>
-  </si>
-  <si>
     <t>Dimension_Distortion</t>
   </si>
   <si>
@@ -580,27 +535,6 @@
     <t>Invincible</t>
   </si>
   <si>
-    <t>전신의 힘을 끌어모아 강력한 일격을 날립니다</t>
-  </si>
-  <si>
-    <t>해머를 올려쳐 적을 공중에 띄웁니다</t>
-  </si>
-  <si>
-    <t>강한 인력을 발생시켜 적들을 끌어 모읍니다</t>
-  </si>
-  <si>
-    <t>해머를 회전시키며 하늘 높이 뛰어올라 번개와 함께 강력한 일격을 날립니다</t>
-  </si>
-  <si>
-    <t>대미지와 관통력을 극단적으로 끌어올린 대신 사거리가 줄어든 탄환을 연속하여 발사합니다</t>
-  </si>
-  <si>
-    <t>지정된 범위에 폭발하는 플라즈마 탄을 발사합니다</t>
-  </si>
-  <si>
-    <t>폭격기를 소환해 지정된 지역에 강력한 폭탄을 투하합니다</t>
-  </si>
-  <si>
     <t>Explanation</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -837,6 +771,87 @@
   <si>
     <t>Skill</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>트와이스 커터</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>라이징 슬래쉬</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>어니스트</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>디멘션 디스토션</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>부스트 해머 일반 공격</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>고르디우스의 바퀴</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>승룡추</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>인력장</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>윤회</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>나락</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>플라즈마 라이플 일반 공격</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PG - 15</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>철갑 사격</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>핀 포인트 다운</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>지정 섬멸</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>전신의 힘을 끌어모아 강력한 일격을 날린다</t>
+  </si>
+  <si>
+    <t>해머를 올려쳐 적을 공중에 띄운다</t>
+  </si>
+  <si>
+    <t>강한 인력을 발생시켜 적들을 끌어 모은다</t>
+  </si>
+  <si>
+    <t>해머를 회전시키며 하늘 높이 뛰어올라 번개와 함께 강력한 일격을 날린다</t>
+  </si>
+  <si>
+    <t>대미지와 관통력을 극단적으로 끌어올린 대신 사거리가 줄어든 탄환을 연속하여 발사한다</t>
+  </si>
+  <si>
+    <t>지정된 범위에 폭발하는 플라즈마 탄을 발사한다</t>
+  </si>
+  <si>
+    <t>폭격기를 소환해 지정된 지역에 강력한 폭탄을 투하한다</t>
   </si>
 </sst>
 </file>
@@ -1877,22 +1892,22 @@
         <v>15</v>
       </c>
       <c r="B1" s="46" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="C1" s="46" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D1" s="46" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="E1" s="46" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="F1" s="46" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="G1" s="62" t="s">
-        <v>227</v>
+        <v>205</v>
       </c>
       <c r="H1" s="62"/>
     </row>
@@ -2205,8 +2220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAE0AA7C-D827-478C-A8E1-4F3353839195}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17"/>
@@ -2225,31 +2240,31 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="57" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
       <c r="B1" s="57" t="s">
         <v>15</v>
       </c>
       <c r="C1" s="57" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="D1" s="57" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
       <c r="E1" s="57" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="F1" s="57" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="G1" s="57" t="s">
-        <v>175</v>
+        <v>153</v>
       </c>
       <c r="H1" s="57" t="s">
-        <v>174</v>
+        <v>152</v>
       </c>
       <c r="I1" s="56" t="s">
-        <v>192</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -2260,10 +2275,10 @@
         <v>2000</v>
       </c>
       <c r="C2" s="58" t="s">
-        <v>176</v>
+        <v>154</v>
       </c>
       <c r="D2" s="58" t="s">
-        <v>177</v>
+        <v>155</v>
       </c>
       <c r="E2" s="59">
         <v>1</v>
@@ -2278,7 +2293,7 @@
         <v>0.1</v>
       </c>
       <c r="I2" s="58" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="J2" s="58"/>
     </row>
@@ -2290,10 +2305,10 @@
         <v>2001</v>
       </c>
       <c r="C3" s="58" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="D3" s="58" t="s">
-        <v>179</v>
+        <v>157</v>
       </c>
       <c r="E3" s="59">
         <v>2</v>
@@ -2308,7 +2323,7 @@
         <v>0.15</v>
       </c>
       <c r="I3" s="58" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
       <c r="J3" s="58"/>
     </row>
@@ -2320,10 +2335,10 @@
         <v>2002</v>
       </c>
       <c r="C4" s="58" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
       <c r="D4" s="58" t="s">
-        <v>181</v>
+        <v>159</v>
       </c>
       <c r="E4" s="59">
         <v>3</v>
@@ -2338,7 +2353,7 @@
         <v>0.2</v>
       </c>
       <c r="I4" s="58" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="J4" s="58"/>
     </row>
@@ -2350,10 +2365,10 @@
         <v>3000</v>
       </c>
       <c r="C5" s="58" t="s">
-        <v>182</v>
+        <v>160</v>
       </c>
       <c r="D5" s="58" t="s">
-        <v>183</v>
+        <v>161</v>
       </c>
       <c r="E5" s="59">
         <v>4</v>
@@ -2368,7 +2383,7 @@
         <v>0.1</v>
       </c>
       <c r="I5" s="58" t="s">
-        <v>193</v>
+        <v>171</v>
       </c>
       <c r="J5" s="58"/>
     </row>
@@ -2380,10 +2395,10 @@
         <v>3001</v>
       </c>
       <c r="C6" s="58" t="s">
-        <v>184</v>
+        <v>162</v>
       </c>
       <c r="D6" s="58" t="s">
-        <v>185</v>
+        <v>163</v>
       </c>
       <c r="E6" s="59">
         <v>5</v>
@@ -2398,7 +2413,7 @@
         <v>0.1</v>
       </c>
       <c r="I6" s="58" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="J6" s="58"/>
     </row>
@@ -2410,10 +2425,10 @@
         <v>3002</v>
       </c>
       <c r="C7" s="58" t="s">
-        <v>186</v>
+        <v>164</v>
       </c>
       <c r="D7" s="58" t="s">
-        <v>187</v>
+        <v>165</v>
       </c>
       <c r="E7" s="59">
         <v>6</v>
@@ -2428,7 +2443,7 @@
         <v>0.02</v>
       </c>
       <c r="I7" s="58" t="s">
-        <v>198</v>
+        <v>176</v>
       </c>
       <c r="J7" s="58"/>
     </row>
@@ -2454,52 +2469,52 @@
         <v>15</v>
       </c>
       <c r="B1" s="49" t="s">
-        <v>209</v>
+        <v>187</v>
       </c>
       <c r="C1" s="49" t="s">
-        <v>210</v>
+        <v>188</v>
       </c>
       <c r="D1" s="49" t="s">
-        <v>211</v>
+        <v>189</v>
       </c>
       <c r="E1" s="49" t="s">
-        <v>212</v>
+        <v>190</v>
       </c>
       <c r="F1" s="49" t="s">
-        <v>213</v>
+        <v>191</v>
       </c>
       <c r="G1" s="49" t="s">
-        <v>214</v>
+        <v>192</v>
       </c>
       <c r="H1" s="49" t="s">
-        <v>215</v>
+        <v>193</v>
       </c>
       <c r="I1" s="49" t="s">
-        <v>216</v>
+        <v>194</v>
       </c>
       <c r="J1" s="49" t="s">
-        <v>217</v>
+        <v>195</v>
       </c>
       <c r="K1" s="49" t="s">
-        <v>218</v>
+        <v>196</v>
       </c>
       <c r="L1" s="49" t="s">
-        <v>219</v>
+        <v>197</v>
       </c>
       <c r="M1" s="49" t="s">
-        <v>220</v>
+        <v>198</v>
       </c>
       <c r="N1" s="49" t="s">
-        <v>221</v>
+        <v>199</v>
       </c>
       <c r="O1" s="49" t="s">
-        <v>222</v>
+        <v>200</v>
       </c>
       <c r="P1" s="49" t="s">
-        <v>223</v>
+        <v>201</v>
       </c>
       <c r="Q1" s="49" t="s">
-        <v>224</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="17.5" thickBot="1">
@@ -2510,49 +2525,49 @@
         <v>3000</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>225</v>
+        <v>203</v>
       </c>
       <c r="D2" s="9">
         <v>0</v>
       </c>
       <c r="E2" s="42" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="F2" s="9">
         <v>0</v>
       </c>
       <c r="G2" s="42" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="H2" s="9">
         <v>0</v>
       </c>
       <c r="I2" s="42" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="J2" s="9">
         <v>0</v>
       </c>
       <c r="K2" s="42" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="L2" s="9">
         <v>0</v>
       </c>
       <c r="M2" s="42" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="N2" s="9">
         <v>0</v>
       </c>
       <c r="O2" s="42" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="P2" s="9">
         <v>0</v>
       </c>
       <c r="Q2" s="42" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -2565,8 +2580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2F9EEC3-3347-4F2E-9FD6-D990126A68DE}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="G8" workbookViewId="0">
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="17"/>
@@ -2579,7 +2594,7 @@
     <col min="9" max="9" width="8.58203125" style="18"/>
     <col min="10" max="10" width="13.75" style="18" customWidth="1"/>
     <col min="11" max="13" width="8.58203125" style="18"/>
-    <col min="14" max="14" width="17" style="18" customWidth="1"/>
+    <col min="14" max="14" width="40.75" style="18" customWidth="1"/>
     <col min="15" max="16384" width="8.58203125" style="18"/>
   </cols>
   <sheetData>
@@ -2612,19 +2627,19 @@
         <v>23</v>
       </c>
       <c r="J1" s="41" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="K1" s="20" t="s">
         <v>24</v>
       </c>
       <c r="L1" s="20" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="M1" s="20" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="N1" s="55" t="s">
-        <v>169</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="34.5" thickBot="1">
@@ -2667,9 +2682,7 @@
       <c r="M2" s="6">
         <v>0</v>
       </c>
-      <c r="N2" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="N2" s="7"/>
     </row>
     <row r="3" spans="1:14" ht="34.5" thickBot="1">
       <c r="A3" s="6">
@@ -2691,11 +2704,11 @@
         <v>2</v>
       </c>
       <c r="G3" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="7" t="s">
-        <v>29</v>
-      </c>
       <c r="I3" s="22" t="b">
         <v>0</v>
       </c>
@@ -2711,9 +2724,7 @@
       <c r="M3" s="6">
         <v>0</v>
       </c>
-      <c r="N3" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="N3" s="7"/>
     </row>
     <row r="4" spans="1:14" ht="17.5" thickBot="1">
       <c r="A4" s="19">
@@ -2735,10 +2746,10 @@
         <v>3</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>30</v>
+        <v>222</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I4" s="23" t="b">
         <v>0</v>
@@ -2755,9 +2766,7 @@
       <c r="M4" s="6">
         <v>0</v>
       </c>
-      <c r="N4" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="N4" s="7"/>
     </row>
     <row r="5" spans="1:14" ht="17.5" thickBot="1">
       <c r="A5" s="6">
@@ -2779,10 +2788,10 @@
         <v>2</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>116</v>
+        <v>223</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="I5" s="22" t="b">
         <v>0</v>
@@ -2799,9 +2808,7 @@
       <c r="M5" s="6">
         <v>0</v>
       </c>
-      <c r="N5" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="N5" s="7"/>
     </row>
     <row r="6" spans="1:14" ht="34.5" thickBot="1">
       <c r="A6" s="6">
@@ -2823,10 +2830,10 @@
         <v>1</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>122</v>
+        <v>224</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="I6" s="22" t="b">
         <v>0</v>
@@ -2843,16 +2850,14 @@
       <c r="M6" s="6">
         <v>0</v>
       </c>
-      <c r="N6" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="N6" s="7"/>
     </row>
     <row r="7" spans="1:14" ht="34.5" thickBot="1">
       <c r="A7" s="6">
         <v>200</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C7" s="6">
         <v>1</v>
@@ -2867,10 +2872,10 @@
         <v>2</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>33</v>
+        <v>225</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I7" s="22" t="b">
         <v>0</v>
@@ -2888,7 +2893,7 @@
         <v>0</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="51.5" thickBot="1">
@@ -2896,7 +2901,7 @@
         <v>201</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C8" s="6">
         <v>2</v>
@@ -2911,10 +2916,10 @@
         <v>3</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>35</v>
+        <v>226</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="I8" s="22" t="b">
         <v>0</v>
@@ -2932,7 +2937,7 @@
         <v>0</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>162</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="34.5" thickBot="1">
@@ -2940,7 +2945,7 @@
         <v>202</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C9" s="6">
         <v>2</v>
@@ -2955,10 +2960,10 @@
         <v>1</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>37</v>
+        <v>227</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="I9" s="22" t="b">
         <v>0</v>
@@ -2976,7 +2981,7 @@
         <v>0</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>163</v>
+        <v>237</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="51.5" thickBot="1">
@@ -2984,7 +2989,7 @@
         <v>203</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C10" s="6">
         <v>2</v>
@@ -2999,10 +3004,10 @@
         <v>3</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>39</v>
+        <v>228</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="I10" s="22" t="b">
         <v>0</v>
@@ -3020,7 +3025,7 @@
         <v>0</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>164</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="68.5" thickBot="1">
@@ -3028,7 +3033,7 @@
         <v>231</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C11" s="6">
         <v>3</v>
@@ -3043,10 +3048,10 @@
         <v>1</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>41</v>
+        <v>229</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="I11" s="22" t="b">
         <v>0</v>
@@ -3064,7 +3069,7 @@
         <v>232</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>165</v>
+        <v>239</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="17.5" thickBot="1">
@@ -3072,7 +3077,7 @@
         <v>232</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C12" s="6">
         <v>3</v>
@@ -3087,10 +3092,10 @@
         <v>2</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>43</v>
+        <v>230</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="I12" s="22" t="b">
         <v>1</v>
@@ -3108,7 +3113,7 @@
         <v>0</v>
       </c>
       <c r="N12" s="7" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="17.5" thickBot="1">
@@ -3116,7 +3121,7 @@
         <v>300</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C13" s="6">
         <v>1</v>
@@ -3131,10 +3136,10 @@
         <v>1</v>
       </c>
       <c r="G13" s="25" t="s">
-        <v>46</v>
+        <v>231</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="I13" s="22" t="b">
         <v>1</v>
@@ -3152,7 +3157,7 @@
         <v>0</v>
       </c>
       <c r="N13" s="7" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="17.5" thickBot="1">
@@ -3160,7 +3165,7 @@
         <v>301</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C14" s="6">
         <v>2</v>
@@ -3175,10 +3180,10 @@
         <v>1</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>48</v>
+        <v>232</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="I14" s="22" t="b">
         <v>0</v>
@@ -3202,7 +3207,7 @@
         <v>302</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C15" s="6">
         <v>2</v>
@@ -3217,10 +3222,10 @@
         <v>1</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>50</v>
+        <v>233</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="I15" s="22" t="b">
         <v>1</v>
@@ -3238,7 +3243,7 @@
         <v>0</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>166</v>
+        <v>240</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="51.5" thickBot="1">
@@ -3246,7 +3251,7 @@
         <v>303</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C16" s="6">
         <v>2</v>
@@ -3261,10 +3266,10 @@
         <v>1</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>52</v>
+        <v>234</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="I16" s="22" t="b">
         <v>1</v>
@@ -3282,7 +3287,7 @@
         <v>0</v>
       </c>
       <c r="N16" s="7" t="s">
-        <v>167</v>
+        <v>241</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="51.5" thickBot="1">
@@ -3290,7 +3295,7 @@
         <v>331</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C17" s="6">
         <v>3</v>
@@ -3305,10 +3310,10 @@
         <v>1</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>54</v>
+        <v>235</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="I17" s="22" t="b">
         <v>1</v>
@@ -3326,7 +3331,7 @@
         <v>0</v>
       </c>
       <c r="N17" s="7" t="s">
-        <v>168</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -3354,49 +3359,49 @@
         <v>15</v>
       </c>
       <c r="B1" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="M1" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="N1" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="O1" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="P1" s="31" t="s">
         <v>57</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="F1" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="G1" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="L1" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="M1" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="N1" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="O1" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="P1" s="31" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -3404,7 +3409,7 @@
         <v>100011101</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C2" s="6">
         <v>1</v>
@@ -3454,7 +3459,7 @@
         <v>100011102</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C3" s="6">
         <v>1</v>
@@ -3504,7 +3509,7 @@
         <v>101012101</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="C4" s="6">
         <v>1</v>
@@ -3554,7 +3559,7 @@
         <v>101012102</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="C5" s="6">
         <v>1</v>
@@ -3604,7 +3609,7 @@
         <v>101012201</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="C6" s="6">
         <v>2</v>
@@ -3654,7 +3659,7 @@
         <v>101012202</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="C7" s="6">
         <v>2</v>
@@ -3704,7 +3709,7 @@
         <v>101012301</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="C8" s="6">
         <v>3</v>
@@ -3754,7 +3759,7 @@
         <v>101012302</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="C9" s="6">
         <v>3</v>
@@ -3804,7 +3809,7 @@
         <v>101012401</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="C10" s="6">
         <v>4</v>
@@ -3854,7 +3859,7 @@
         <v>101012402</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="C11" s="6">
         <v>4</v>
@@ -3904,7 +3909,7 @@
         <v>101012501</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="C12" s="6">
         <v>5</v>
@@ -3954,7 +3959,7 @@
         <v>101012502</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="C13" s="6">
         <v>5</v>
@@ -4004,7 +4009,7 @@
         <v>102012101</v>
       </c>
       <c r="B14" s="33" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C14" s="33">
         <v>1</v>
@@ -4054,7 +4059,7 @@
         <v>102012102</v>
       </c>
       <c r="B15" s="36" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C15" s="36">
         <v>1</v>
@@ -4104,7 +4109,7 @@
         <v>102012103</v>
       </c>
       <c r="B16" s="36" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C16" s="36">
         <v>1</v>
@@ -4154,7 +4159,7 @@
         <v>102012201</v>
       </c>
       <c r="B17" s="36" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C17" s="36">
         <v>2</v>
@@ -4204,7 +4209,7 @@
         <v>102012202</v>
       </c>
       <c r="B18" s="36" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C18" s="36">
         <v>2</v>
@@ -4254,7 +4259,7 @@
         <v>102012203</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C19" s="36">
         <v>2</v>
@@ -4304,7 +4309,7 @@
         <v>102012301</v>
       </c>
       <c r="B20" s="36" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C20" s="36">
         <v>3</v>
@@ -4354,7 +4359,7 @@
         <v>102012302</v>
       </c>
       <c r="B21" s="36" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C21" s="36">
         <v>3</v>
@@ -4404,7 +4409,7 @@
         <v>102012303</v>
       </c>
       <c r="B22" s="36" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C22" s="36">
         <v>3</v>
@@ -4454,7 +4459,7 @@
         <v>102012401</v>
       </c>
       <c r="B23" s="36" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C23" s="36">
         <v>4</v>
@@ -4504,7 +4509,7 @@
         <v>102012402</v>
       </c>
       <c r="B24" s="36" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C24" s="36">
         <v>4</v>
@@ -4554,7 +4559,7 @@
         <v>102012403</v>
       </c>
       <c r="B25" s="36" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C25" s="36">
         <v>4</v>
@@ -4604,7 +4609,7 @@
         <v>102012501</v>
       </c>
       <c r="B26" s="36" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C26" s="36">
         <v>5</v>
@@ -4654,7 +4659,7 @@
         <v>102012502</v>
       </c>
       <c r="B27" s="36" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C27" s="36">
         <v>5</v>
@@ -4704,7 +4709,7 @@
         <v>102012503</v>
       </c>
       <c r="B28" s="39" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C28" s="39">
         <v>5</v>
@@ -4754,7 +4759,7 @@
         <v>103012101</v>
       </c>
       <c r="B29" s="42" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="C29" s="9">
         <v>1</v>
@@ -4804,7 +4809,7 @@
         <v>103012102</v>
       </c>
       <c r="B30" s="42" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="C30" s="9">
         <v>1</v>
@@ -4854,7 +4859,7 @@
         <v>103012103</v>
       </c>
       <c r="B31" s="42" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="C31" s="9">
         <v>1</v>
@@ -4904,7 +4909,7 @@
         <v>103012104</v>
       </c>
       <c r="B32" s="42" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="C32" s="9">
         <v>1</v>
@@ -4954,7 +4959,7 @@
         <v>103012201</v>
       </c>
       <c r="B33" s="42" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="C33" s="9">
         <v>2</v>
@@ -5004,7 +5009,7 @@
         <v>103012202</v>
       </c>
       <c r="B34" s="42" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="C34" s="9">
         <v>2</v>
@@ -5054,7 +5059,7 @@
         <v>103012203</v>
       </c>
       <c r="B35" s="42" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="C35" s="9">
         <v>2</v>
@@ -5104,7 +5109,7 @@
         <v>103012204</v>
       </c>
       <c r="B36" s="42" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="C36" s="9">
         <v>2</v>
@@ -5154,7 +5159,7 @@
         <v>103012301</v>
       </c>
       <c r="B37" s="42" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="C37" s="9">
         <v>3</v>
@@ -5204,7 +5209,7 @@
         <v>103012302</v>
       </c>
       <c r="B38" s="42" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="C38" s="9">
         <v>3</v>
@@ -5254,7 +5259,7 @@
         <v>103012303</v>
       </c>
       <c r="B39" s="42" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="C39" s="9">
         <v>3</v>
@@ -5304,7 +5309,7 @@
         <v>103012304</v>
       </c>
       <c r="B40" s="42" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="C40" s="9">
         <v>3</v>
@@ -5354,7 +5359,7 @@
         <v>103012401</v>
       </c>
       <c r="B41" s="42" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="C41" s="9">
         <v>4</v>
@@ -5404,7 +5409,7 @@
         <v>103012402</v>
       </c>
       <c r="B42" s="42" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="C42" s="9">
         <v>4</v>
@@ -5454,7 +5459,7 @@
         <v>103012403</v>
       </c>
       <c r="B43" s="42" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="C43" s="9">
         <v>4</v>
@@ -5504,7 +5509,7 @@
         <v>103012404</v>
       </c>
       <c r="B44" s="42" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="C44" s="9">
         <v>4</v>
@@ -5554,7 +5559,7 @@
         <v>103012501</v>
       </c>
       <c r="B45" s="42" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="C45" s="9">
         <v>5</v>
@@ -5604,7 +5609,7 @@
         <v>103012502</v>
       </c>
       <c r="B46" s="42" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="C46" s="9">
         <v>5</v>
@@ -5654,7 +5659,7 @@
         <v>103012503</v>
       </c>
       <c r="B47" s="42" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="C47" s="9">
         <v>5</v>
@@ -5704,7 +5709,7 @@
         <v>103012504</v>
       </c>
       <c r="B48" s="42" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="C48" s="9">
         <v>5</v>
@@ -5754,7 +5759,7 @@
         <v>131013101</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C49" s="6">
         <v>1</v>
@@ -5814,7 +5819,7 @@
         <v>131013201</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C50" s="6">
         <v>2</v>
@@ -5874,7 +5879,7 @@
         <v>131013301</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C51" s="6">
         <v>3</v>
@@ -5934,7 +5939,7 @@
         <v>200021101</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C52" s="6">
         <v>1</v>
@@ -5984,7 +5989,7 @@
         <v>200021102</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C53" s="6">
         <v>1</v>
@@ -6034,7 +6039,7 @@
         <v>201022101</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C54" s="6">
         <v>1</v>
@@ -6084,7 +6089,7 @@
         <v>201022102</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C55" s="6">
         <v>1</v>
@@ -6134,7 +6139,7 @@
         <v>201022201</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C56" s="6">
         <v>2</v>
@@ -6184,7 +6189,7 @@
         <v>201022202</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C57" s="6">
         <v>2</v>
@@ -6234,7 +6239,7 @@
         <v>201022301</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C58" s="6">
         <v>3</v>
@@ -6284,7 +6289,7 @@
         <v>201022302</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C59" s="6">
         <v>3</v>
@@ -6334,7 +6339,7 @@
         <v>201022401</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C60" s="6">
         <v>4</v>
@@ -6384,7 +6389,7 @@
         <v>201022402</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C61" s="6">
         <v>4</v>
@@ -6434,7 +6439,7 @@
         <v>201022501</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C62" s="6">
         <v>5</v>
@@ -6484,7 +6489,7 @@
         <v>201022502</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C63" s="6">
         <v>5</v>
@@ -6534,7 +6539,7 @@
         <v>201022111</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C64" s="6">
         <v>1</v>
@@ -6584,7 +6589,7 @@
         <v>201022112</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C65" s="6">
         <v>1</v>
@@ -6634,7 +6639,7 @@
         <v>201022211</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C66" s="6">
         <v>2</v>
@@ -6684,7 +6689,7 @@
         <v>201022212</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C67" s="6">
         <v>2</v>
@@ -6734,7 +6739,7 @@
         <v>201022311</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C68" s="6">
         <v>3</v>
@@ -6784,7 +6789,7 @@
         <v>201022312</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C69" s="6">
         <v>3</v>
@@ -6834,7 +6839,7 @@
         <v>201022411</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C70" s="6">
         <v>4</v>
@@ -6884,7 +6889,7 @@
         <v>201022412</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C71" s="6">
         <v>4</v>
@@ -6934,7 +6939,7 @@
         <v>201022511</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C72" s="6">
         <v>5</v>
@@ -6984,7 +6989,7 @@
         <v>201022512</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C73" s="6">
         <v>5</v>
@@ -7034,7 +7039,7 @@
         <v>201022121</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C74" s="6">
         <v>1</v>
@@ -7084,7 +7089,7 @@
         <v>201022122</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C75" s="6">
         <v>1</v>
@@ -7134,7 +7139,7 @@
         <v>201022123</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C76" s="6">
         <v>1</v>
@@ -7184,7 +7189,7 @@
         <v>201022221</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C77" s="6">
         <v>2</v>
@@ -7234,7 +7239,7 @@
         <v>201022222</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C78" s="6">
         <v>2</v>
@@ -7284,7 +7289,7 @@
         <v>201022223</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C79" s="6">
         <v>2</v>
@@ -7334,7 +7339,7 @@
         <v>201022321</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C80" s="6">
         <v>3</v>
@@ -7384,7 +7389,7 @@
         <v>201022322</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C81" s="6">
         <v>3</v>
@@ -7434,7 +7439,7 @@
         <v>201022323</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C82" s="6">
         <v>3</v>
@@ -7484,7 +7489,7 @@
         <v>201022421</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C83" s="6">
         <v>4</v>
@@ -7534,7 +7539,7 @@
         <v>201022422</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C84" s="6">
         <v>4</v>
@@ -7584,7 +7589,7 @@
         <v>201022423</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C85" s="6">
         <v>4</v>
@@ -7634,7 +7639,7 @@
         <v>201022521</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C86" s="6">
         <v>5</v>
@@ -7684,7 +7689,7 @@
         <v>201022522</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C87" s="6">
         <v>5</v>
@@ -7734,7 +7739,7 @@
         <v>201022523</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C88" s="6">
         <v>5</v>
@@ -7784,7 +7789,7 @@
         <v>202022101</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C89" s="6">
         <v>1</v>
@@ -7834,7 +7839,7 @@
         <v>202022201</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C90" s="6">
         <v>2</v>
@@ -7884,7 +7889,7 @@
         <v>202022301</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C91" s="6">
         <v>3</v>
@@ -7934,7 +7939,7 @@
         <v>202022401</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C92" s="6">
         <v>4</v>
@@ -7984,7 +7989,7 @@
         <v>202022501</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C93" s="6">
         <v>5</v>
@@ -8034,7 +8039,7 @@
         <v>203022101</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C94" s="6">
         <v>1</v>
@@ -8084,7 +8089,7 @@
         <v>203022102</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C95" s="6">
         <v>1</v>
@@ -8134,7 +8139,7 @@
         <v>203022103</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C96" s="6">
         <v>1</v>
@@ -8184,7 +8189,7 @@
         <v>203022201</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C97" s="6">
         <v>2</v>
@@ -8234,7 +8239,7 @@
         <v>203022202</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C98" s="6">
         <v>2</v>
@@ -8284,7 +8289,7 @@
         <v>203022203</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C99" s="6">
         <v>2</v>
@@ -8334,7 +8339,7 @@
         <v>203022301</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C100" s="6">
         <v>3</v>
@@ -8384,7 +8389,7 @@
         <v>203022302</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C101" s="6">
         <v>3</v>
@@ -8434,7 +8439,7 @@
         <v>203022303</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C102" s="6">
         <v>3</v>
@@ -8484,7 +8489,7 @@
         <v>203022401</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C103" s="6">
         <v>4</v>
@@ -8534,7 +8539,7 @@
         <v>203022402</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C104" s="6">
         <v>4</v>
@@ -8584,7 +8589,7 @@
         <v>203022403</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C105" s="6">
         <v>4</v>
@@ -8634,7 +8639,7 @@
         <v>203022501</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C106" s="6">
         <v>5</v>
@@ -8684,7 +8689,7 @@
         <v>203022502</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C107" s="6">
         <v>5</v>
@@ -8734,7 +8739,7 @@
         <v>203022503</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C108" s="6">
         <v>5</v>
@@ -8784,7 +8789,7 @@
         <v>231023101</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="C109" s="6">
         <v>1</v>
@@ -8834,7 +8839,7 @@
         <v>231023201</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="C110" s="6">
         <v>2</v>
@@ -8884,7 +8889,7 @@
         <v>231023301</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="C111" s="6">
         <v>3</v>
@@ -8934,7 +8939,7 @@
         <v>232023101</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C112" s="6">
         <v>1</v>
@@ -8984,7 +8989,7 @@
         <v>232023102</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C113" s="6">
         <v>1</v>
@@ -9034,7 +9039,7 @@
         <v>232023201</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C114" s="6">
         <v>2</v>
@@ -9084,7 +9089,7 @@
         <v>232023202</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C115" s="6">
         <v>2</v>
@@ -9134,7 +9139,7 @@
         <v>232023301</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C116" s="6">
         <v>3</v>
@@ -9184,7 +9189,7 @@
         <v>232023302</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C117" s="6">
         <v>3</v>
@@ -9234,7 +9239,7 @@
         <v>300031101</v>
       </c>
       <c r="B118" s="44" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C118" s="1">
         <v>1</v>
@@ -9284,7 +9289,7 @@
         <v>301032101</v>
       </c>
       <c r="B119" s="44" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="C119" s="1">
         <v>1</v>
@@ -9334,7 +9339,7 @@
         <v>301032201</v>
       </c>
       <c r="B120" s="44" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="C120" s="1">
         <v>2</v>
@@ -9384,7 +9389,7 @@
         <v>301032301</v>
       </c>
       <c r="B121" s="44" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="C121" s="1">
         <v>3</v>
@@ -9434,7 +9439,7 @@
         <v>301032401</v>
       </c>
       <c r="B122" s="44" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="C122" s="1">
         <v>4</v>
@@ -9484,7 +9489,7 @@
         <v>301032501</v>
       </c>
       <c r="B123" s="44" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="C123" s="1">
         <v>5</v>
@@ -9534,7 +9539,7 @@
         <v>302032101</v>
       </c>
       <c r="B124" s="44" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C124" s="1">
         <v>1</v>
@@ -9584,7 +9589,7 @@
         <v>302032201</v>
       </c>
       <c r="B125" s="44" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C125" s="1">
         <v>2</v>
@@ -9634,7 +9639,7 @@
         <v>302032301</v>
       </c>
       <c r="B126" s="44" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C126" s="1">
         <v>3</v>
@@ -9684,7 +9689,7 @@
         <v>302032401</v>
       </c>
       <c r="B127" s="44" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C127" s="1">
         <v>4</v>
@@ -9734,7 +9739,7 @@
         <v>302032501</v>
       </c>
       <c r="B128" s="44" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C128" s="1">
         <v>5</v>
@@ -9784,7 +9789,7 @@
         <v>303032101</v>
       </c>
       <c r="B129" s="44" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C129" s="1">
         <v>1</v>
@@ -9834,7 +9839,7 @@
         <v>303032102</v>
       </c>
       <c r="B130" s="44" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C130" s="1">
         <v>1</v>
@@ -9884,7 +9889,7 @@
         <v>303032201</v>
       </c>
       <c r="B131" s="44" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C131" s="1">
         <v>2</v>
@@ -9934,7 +9939,7 @@
         <v>303032202</v>
       </c>
       <c r="B132" s="44" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C132" s="1">
         <v>2</v>
@@ -9984,7 +9989,7 @@
         <v>303032301</v>
       </c>
       <c r="B133" s="44" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C133" s="1">
         <v>3</v>
@@ -10034,7 +10039,7 @@
         <v>303032302</v>
       </c>
       <c r="B134" s="44" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C134" s="1">
         <v>3</v>
@@ -10084,7 +10089,7 @@
         <v>303032401</v>
       </c>
       <c r="B135" s="44" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C135" s="1">
         <v>4</v>
@@ -10134,7 +10139,7 @@
         <v>303032402</v>
       </c>
       <c r="B136" s="44" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C136" s="1">
         <v>4</v>
@@ -10184,7 +10189,7 @@
         <v>303032501</v>
       </c>
       <c r="B137" s="44" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C137" s="1">
         <v>5</v>
@@ -10234,7 +10239,7 @@
         <v>303032502</v>
       </c>
       <c r="B138" s="44" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C138" s="1">
         <v>5</v>
@@ -10284,7 +10289,7 @@
         <v>331033101</v>
       </c>
       <c r="B139" s="44" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C139" s="1">
         <v>1</v>
@@ -10334,7 +10339,7 @@
         <v>331033201</v>
       </c>
       <c r="B140" s="44" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C140" s="1">
         <v>2</v>
@@ -10384,7 +10389,7 @@
         <v>331033301</v>
       </c>
       <c r="B141" s="44" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C141" s="1">
         <v>3</v>
@@ -10454,19 +10459,19 @@
         <v>15</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="17.5" thickBot="1">
@@ -10822,52 +10827,52 @@
         <v>15</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="C1" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="N1" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="O1" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="P1" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="N1" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="O1" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="P1" s="16" t="s">
-        <v>97</v>
-      </c>
       <c r="Q1" s="14" t="s">
-        <v>242</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="17.5" thickBot="1">
@@ -10881,7 +10886,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>226</v>
+        <v>204</v>
       </c>
       <c r="E2" s="6" t="b">
         <v>0</v>
@@ -10934,7 +10939,7 @@
         <v>30</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="E3" s="6" t="b">
         <v>1</v>
@@ -10987,7 +10992,7 @@
         <v>20</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="E4" s="6" t="b">
         <v>0</v>
@@ -11040,7 +11045,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="E5" s="6" t="b">
         <v>0</v>
@@ -11100,46 +11105,46 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="B1" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="C1" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="D1" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="E1" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="F1" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="G1" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="H1" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="I1" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="J1" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="K1" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="L1" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="M1" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="N1" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -11210,70 +11215,70 @@
         <v>15</v>
       </c>
       <c r="B1" s="46" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="C1" s="51" t="s">
         <v>17</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="E1" s="50" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="F1" s="50" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="G1" s="48" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="H1" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1" s="48" t="s">
         <v>90</v>
       </c>
-      <c r="I1" s="48" t="s">
-        <v>103</v>
-      </c>
       <c r="J1" s="48" t="s">
+        <v>79</v>
+      </c>
+      <c r="K1" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="L1" s="48" t="s">
+        <v>81</v>
+      </c>
+      <c r="M1" s="47" t="s">
+        <v>91</v>
+      </c>
+      <c r="N1" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="K1" s="48" t="s">
+      <c r="O1" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="L1" s="48" t="s">
+      <c r="P1" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="M1" s="47" t="s">
-        <v>104</v>
-      </c>
-      <c r="N1" s="47" t="s">
-        <v>105</v>
-      </c>
-      <c r="O1" s="47" t="s">
-        <v>106</v>
-      </c>
-      <c r="P1" s="47" t="s">
-        <v>107</v>
-      </c>
       <c r="Q1" s="47" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="R1" s="47" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="S1" s="49" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="T1" s="53" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="U1" s="60" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="V1" s="49" t="s">
-        <v>205</v>
+        <v>183</v>
       </c>
       <c r="W1" s="49" t="s">
-        <v>206</v>
+        <v>184</v>
       </c>
       <c r="X1" s="49"/>
       <c r="Y1" s="49"/>
@@ -11297,13 +11302,13 @@
         <v>1000</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="C2" s="9">
         <v>1</v>
       </c>
       <c r="D2" s="42" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="E2" s="9">
         <v>150</v>
@@ -11384,13 +11389,13 @@
         <v>1001</v>
       </c>
       <c r="B3" s="42" t="s">
-        <v>188</v>
+        <v>166</v>
       </c>
       <c r="C3" s="9">
         <v>1</v>
       </c>
       <c r="D3" s="42" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="E3" s="9">
         <v>200</v>
@@ -11471,13 +11476,13 @@
         <v>1002</v>
       </c>
       <c r="B4" s="42" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
       <c r="C4" s="9">
         <v>1</v>
       </c>
       <c r="D4" s="42" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="E4" s="9">
         <v>250</v>
@@ -11558,13 +11563,13 @@
         <v>2000</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="C5" s="9">
         <v>2</v>
       </c>
       <c r="D5" s="42" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="E5" s="9">
         <v>700</v>
@@ -11645,13 +11650,13 @@
         <v>2001</v>
       </c>
       <c r="B6" s="42" t="s">
-        <v>190</v>
+        <v>168</v>
       </c>
       <c r="C6" s="9">
         <v>2</v>
       </c>
       <c r="D6" s="42" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="E6" s="9">
         <v>800</v>
@@ -11732,13 +11737,13 @@
         <v>2002</v>
       </c>
       <c r="B7" s="42" t="s">
-        <v>199</v>
+        <v>177</v>
       </c>
       <c r="C7" s="9">
         <v>2</v>
       </c>
       <c r="D7" s="42" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="E7" s="9">
         <v>900</v>
@@ -11819,13 +11824,13 @@
         <v>3000</v>
       </c>
       <c r="B8" s="42" t="s">
-        <v>200</v>
+        <v>178</v>
       </c>
       <c r="C8" s="9">
         <v>3</v>
       </c>
       <c r="D8" s="42" t="s">
-        <v>201</v>
+        <v>179</v>
       </c>
       <c r="E8" s="9">
         <v>4000</v>
@@ -11906,13 +11911,13 @@
         <v>3001</v>
       </c>
       <c r="B9" s="42" t="s">
-        <v>202</v>
+        <v>180</v>
       </c>
       <c r="C9" s="9">
         <v>3</v>
       </c>
       <c r="D9" s="42" t="s">
-        <v>201</v>
+        <v>179</v>
       </c>
       <c r="E9" s="9">
         <v>8000</v>
@@ -11993,13 +11998,13 @@
         <v>3002</v>
       </c>
       <c r="B10" s="42" t="s">
-        <v>203</v>
+        <v>181</v>
       </c>
       <c r="C10" s="9">
         <v>3</v>
       </c>
       <c r="D10" s="42" t="s">
-        <v>201</v>
+        <v>179</v>
       </c>
       <c r="E10" s="9">
         <v>5000</v>
@@ -12080,13 +12085,13 @@
         <v>3003</v>
       </c>
       <c r="B11" s="42" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="C11" s="9">
         <v>3</v>
       </c>
       <c r="D11" s="42" t="s">
-        <v>201</v>
+        <v>179</v>
       </c>
       <c r="E11" s="9">
         <v>10000</v>
@@ -12167,13 +12172,13 @@
         <v>4000</v>
       </c>
       <c r="B12" s="42" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="C12" s="9">
         <v>4</v>
       </c>
       <c r="D12" s="42" t="s">
-        <v>208</v>
+        <v>186</v>
       </c>
       <c r="E12" s="9">
         <v>15000</v>
@@ -12276,31 +12281,31 @@
         <v>15</v>
       </c>
       <c r="B1" s="46" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="C1" s="47" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="D1" s="48" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="E1" s="48" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="F1" s="49" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="G1" s="49" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="H1" s="49" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="I1" s="49" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="J1" s="50" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="51.5" thickBot="1">
@@ -12308,7 +12313,7 @@
         <v>100000</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>228</v>
+        <v>206</v>
       </c>
       <c r="C2" s="9">
         <v>1</v>
@@ -12332,7 +12337,7 @@
         <v>0</v>
       </c>
       <c r="J2" s="42" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="51.5" thickBot="1">
@@ -12340,7 +12345,7 @@
         <v>200000</v>
       </c>
       <c r="B3" s="42" t="s">
-        <v>229</v>
+        <v>207</v>
       </c>
       <c r="C3" s="9">
         <v>1</v>
@@ -12364,7 +12369,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="42" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="34.5" thickBot="1">
@@ -12372,7 +12377,7 @@
         <v>300000</v>
       </c>
       <c r="B4" s="42" t="s">
-        <v>230</v>
+        <v>208</v>
       </c>
       <c r="C4" s="9">
         <v>2</v>
@@ -12396,7 +12401,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="42" t="s">
-        <v>231</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="34.5" thickBot="1">
@@ -12404,7 +12409,7 @@
         <v>300001</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>230</v>
+        <v>208</v>
       </c>
       <c r="C5" s="9">
         <v>4</v>
@@ -12428,7 +12433,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="42" t="s">
-        <v>232</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="34.5" thickBot="1">
@@ -12436,7 +12441,7 @@
         <v>300002</v>
       </c>
       <c r="B6" s="42" t="s">
-        <v>230</v>
+        <v>208</v>
       </c>
       <c r="C6" s="9">
         <v>4</v>
@@ -12460,7 +12465,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="42" t="s">
-        <v>233</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="34.5" thickBot="1">
@@ -12468,7 +12473,7 @@
         <v>300003</v>
       </c>
       <c r="B7" s="42" t="s">
-        <v>230</v>
+        <v>208</v>
       </c>
       <c r="C7" s="9">
         <v>4</v>
@@ -12492,7 +12497,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="42" t="s">
-        <v>234</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="34.5" thickBot="1">
@@ -12500,7 +12505,7 @@
         <v>300004</v>
       </c>
       <c r="B8" s="42" t="s">
-        <v>230</v>
+        <v>208</v>
       </c>
       <c r="C8" s="9">
         <v>3</v>
@@ -12524,7 +12529,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="42" t="s">
-        <v>235</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="34.5" thickBot="1">
@@ -12532,7 +12537,7 @@
         <v>300005</v>
       </c>
       <c r="B9" s="42" t="s">
-        <v>230</v>
+        <v>208</v>
       </c>
       <c r="C9" s="9">
         <v>1</v>
@@ -12556,7 +12561,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="42" t="s">
-        <v>236</v>
+        <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="34.5" thickBot="1">
@@ -12564,7 +12569,7 @@
         <v>300006</v>
       </c>
       <c r="B10" s="42" t="s">
-        <v>230</v>
+        <v>208</v>
       </c>
       <c r="C10" s="9">
         <v>1</v>
@@ -12588,7 +12593,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="42" t="s">
-        <v>237</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="34.5" thickBot="1">
@@ -12596,7 +12601,7 @@
         <v>300008</v>
       </c>
       <c r="B11" s="42" t="s">
-        <v>230</v>
+        <v>208</v>
       </c>
       <c r="C11" s="9">
         <v>1</v>
@@ -12620,7 +12625,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="42" t="s">
-        <v>238</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="34.5" thickBot="1">
@@ -12628,7 +12633,7 @@
         <v>300009</v>
       </c>
       <c r="B12" s="42" t="s">
-        <v>230</v>
+        <v>208</v>
       </c>
       <c r="C12" s="9">
         <v>2</v>
@@ -12652,7 +12657,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="42" t="s">
-        <v>239</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="34.5" thickBot="1">
@@ -12660,7 +12665,7 @@
         <v>300010</v>
       </c>
       <c r="B13" s="42" t="s">
-        <v>230</v>
+        <v>208</v>
       </c>
       <c r="C13" s="9">
         <v>5</v>
@@ -12684,7 +12689,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="42" t="s">
-        <v>240</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="34.5" thickBot="1">
@@ -12692,7 +12697,7 @@
         <v>300011</v>
       </c>
       <c r="B14" s="42" t="s">
-        <v>230</v>
+        <v>208</v>
       </c>
       <c r="C14" s="9">
         <v>3</v>
@@ -12716,7 +12721,7 @@
         <v>0</v>
       </c>
       <c r="J14" s="42" t="s">
-        <v>241</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -12747,40 +12752,40 @@
         <v>15</v>
       </c>
       <c r="B1" s="51" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="C1" s="48" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="D1" s="48" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="E1" s="48" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="F1" s="48" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="G1" s="48" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="H1" s="48" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="I1" s="52" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="J1" s="47" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="K1" s="47" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="L1" s="47" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="M1" s="53" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="N1" s="18"/>
     </row>
@@ -12789,7 +12794,7 @@
         <v>1000001</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C2" s="9">
         <v>1</v>
@@ -12831,7 +12836,7 @@
         <v>2000001</v>
       </c>
       <c r="B3" s="42" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C3" s="9">
         <v>1</v>
@@ -12873,7 +12878,7 @@
         <v>3000001</v>
       </c>
       <c r="B4" s="42" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C4" s="9">
         <v>1</v>
@@ -12914,7 +12919,7 @@
         <v>3000002</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C5" s="9">
         <v>1</v>
@@ -12955,7 +12960,7 @@
         <v>3000011</v>
       </c>
       <c r="B6" s="42" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C6" s="9">
         <v>1</v>
@@ -12996,7 +13001,7 @@
         <v>3000012</v>
       </c>
       <c r="B7" s="42" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C7" s="9">
         <v>1</v>
@@ -13037,7 +13042,7 @@
         <v>3000013</v>
       </c>
       <c r="B8" s="42" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C8" s="9">
         <v>2</v>
@@ -13078,7 +13083,7 @@
         <v>3000014</v>
       </c>
       <c r="B9" s="42" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C9" s="9">
         <v>1.5</v>
@@ -13119,7 +13124,7 @@
         <v>3000021</v>
       </c>
       <c r="B10" s="42" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C10" s="9">
         <v>1</v>
@@ -13160,7 +13165,7 @@
         <v>3000022</v>
       </c>
       <c r="B11" s="42" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C11" s="9">
         <v>1</v>
@@ -13201,7 +13206,7 @@
         <v>3000023</v>
       </c>
       <c r="B12" s="42" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C12" s="9">
         <v>1</v>
@@ -13242,7 +13247,7 @@
         <v>3000024</v>
       </c>
       <c r="B13" s="42" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C13" s="9">
         <v>1</v>
@@ -13283,7 +13288,7 @@
         <v>3000031</v>
       </c>
       <c r="B14" s="42" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C14" s="9">
         <v>1</v>
@@ -13324,7 +13329,7 @@
         <v>3000032</v>
       </c>
       <c r="B15" s="42" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C15" s="9">
         <v>1</v>
@@ -13365,7 +13370,7 @@
         <v>3000033</v>
       </c>
       <c r="B16" s="42" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C16" s="9">
         <v>1</v>
@@ -13406,7 +13411,7 @@
         <v>3000034</v>
       </c>
       <c r="B17" s="42" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C17" s="9">
         <v>1.5</v>
@@ -13447,7 +13452,7 @@
         <v>3000041</v>
       </c>
       <c r="B18" s="42" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C18" s="9">
         <v>1</v>
@@ -13488,7 +13493,7 @@
         <v>3000042</v>
       </c>
       <c r="B19" s="42" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C19" s="9">
         <v>1</v>
@@ -13529,7 +13534,7 @@
         <v>3000043</v>
       </c>
       <c r="B20" s="42" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C20" s="9">
         <v>2.5</v>
@@ -13570,7 +13575,7 @@
         <v>3000051</v>
       </c>
       <c r="B21" s="42" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C21" s="9">
         <v>0.8</v>
@@ -13611,7 +13616,7 @@
         <v>3000061</v>
       </c>
       <c r="B22" s="42" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C22" s="9">
         <v>1.2</v>
@@ -13652,7 +13657,7 @@
         <v>3000081</v>
       </c>
       <c r="B23" s="42" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C23" s="9">
         <v>2</v>
@@ -13693,7 +13698,7 @@
         <v>3000091</v>
       </c>
       <c r="B24" s="42" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C24" s="9">
         <v>2</v>
@@ -13734,7 +13739,7 @@
         <v>3000092</v>
       </c>
       <c r="B25" s="42" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C25" s="9">
         <v>1.5</v>
@@ -13775,7 +13780,7 @@
         <v>3000101</v>
       </c>
       <c r="B26" s="42" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C26" s="9">
         <v>2</v>
@@ -13816,7 +13821,7 @@
         <v>3000102</v>
       </c>
       <c r="B27" s="42" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C27" s="9">
         <v>2</v>
@@ -13857,7 +13862,7 @@
         <v>3000103</v>
       </c>
       <c r="B28" s="42" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C28" s="9">
         <v>2</v>
@@ -13898,7 +13903,7 @@
         <v>3000104</v>
       </c>
       <c r="B29" s="42" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C29" s="9">
         <v>2</v>
@@ -13939,7 +13944,7 @@
         <v>3000105</v>
       </c>
       <c r="B30" s="42" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C30" s="9">
         <v>3</v>
@@ -13980,7 +13985,7 @@
         <v>3000111</v>
       </c>
       <c r="B31" s="42" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C31" s="9">
         <v>2.5</v>
@@ -14021,7 +14026,7 @@
         <v>3000112</v>
       </c>
       <c r="B32" s="42" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C32" s="9">
         <v>2.5</v>
@@ -14062,7 +14067,7 @@
         <v>3000113</v>
       </c>
       <c r="B33" s="42" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C33" s="9">
         <v>3</v>

</xml_diff>

<commit_message>
ui & pattern & table data
</commit_message>
<xml_diff>
--- a/Assets/04Table/TS.xlsx
+++ b/Assets/04Table/TS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cksgm\Unity\ProjectTS\Assets\04Table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E39008-57AD-446F-99BB-F8EF7991A66C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D3EF59-8289-4310-93D3-0AA98DAF22E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="13770" firstSheet="12" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="13770" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Player_Stats" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="265">
   <si>
     <t>Level</t>
   </si>
@@ -319,15 +319,6 @@
     <t>Attack_Speed</t>
   </si>
   <si>
-    <t>Slash</t>
-  </si>
-  <si>
-    <t>Strike</t>
-  </si>
-  <si>
-    <t>Thrust</t>
-  </si>
-  <si>
     <t>Name</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -599,9 +590,6 @@
     <t>카타안킬로 V2</t>
   </si>
   <si>
-    <t>카타안킬로 V3</t>
-  </si>
-  <si>
     <t>듀리노 V2</t>
   </si>
   <si>
@@ -636,22 +624,10 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>듀리노 V3</t>
-  </si>
-  <si>
     <t>필 데빌 V1</t>
   </si>
   <si>
     <t>무리어미</t>
-  </si>
-  <si>
-    <t>필 데빌 V2</t>
-  </si>
-  <si>
-    <t>시저스도라 V1</t>
-  </si>
-  <si>
-    <t>시저스도라 V2</t>
   </si>
   <si>
     <t>Groggy_HP</t>
@@ -721,15 +697,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>1000, 1001, 1002</t>
-  </si>
-  <si>
-    <t>2000, 2001, 2002</t>
-  </si>
-  <si>
-    <t>3000, 3001</t>
-  </si>
-  <si>
     <t>BothHandSwing</t>
   </si>
   <si>
@@ -935,6 +902,34 @@
   </si>
   <si>
     <t>M_04_Percent</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1000, 1001</t>
+  </si>
+  <si>
+    <t>2000, 2001</t>
+  </si>
+  <si>
+    <t>참격</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>타격</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>관통</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>기본 지급 차지드 소드</t>
+  </si>
+  <si>
+    <t>기본 지급 부스트 해머</t>
+  </si>
+  <si>
+    <t>기본 지급 플라즈마 라이플</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1994,7 +1989,7 @@
         <v>70</v>
       </c>
       <c r="G1" s="55" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="H1" s="55"/>
     </row>
@@ -2327,31 +2322,31 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="50" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B1" s="50" t="s">
         <v>15</v>
       </c>
       <c r="C1" s="50" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D1" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="E1" s="50" t="s">
+        <v>145</v>
+      </c>
+      <c r="F1" s="50" t="s">
+        <v>147</v>
+      </c>
+      <c r="G1" s="50" t="s">
         <v>149</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="H1" s="50" t="s">
         <v>148</v>
       </c>
-      <c r="F1" s="50" t="s">
-        <v>150</v>
-      </c>
-      <c r="G1" s="50" t="s">
-        <v>152</v>
-      </c>
-      <c r="H1" s="50" t="s">
-        <v>151</v>
-      </c>
       <c r="I1" s="49" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -2362,10 +2357,10 @@
         <v>2000</v>
       </c>
       <c r="C2" s="51" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D2" s="51" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E2" s="52">
         <v>1</v>
@@ -2380,7 +2375,7 @@
         <v>0.1</v>
       </c>
       <c r="I2" s="51" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="J2" s="51"/>
     </row>
@@ -2392,10 +2387,10 @@
         <v>2001</v>
       </c>
       <c r="C3" s="51" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D3" s="51" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E3" s="52">
         <v>2</v>
@@ -2410,7 +2405,7 @@
         <v>0.15</v>
       </c>
       <c r="I3" s="51" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="J3" s="51"/>
     </row>
@@ -2422,10 +2417,10 @@
         <v>2002</v>
       </c>
       <c r="C4" s="51" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D4" s="51" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E4" s="52">
         <v>3</v>
@@ -2440,7 +2435,7 @@
         <v>0.2</v>
       </c>
       <c r="I4" s="51" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="J4" s="51"/>
     </row>
@@ -2452,10 +2447,10 @@
         <v>3000</v>
       </c>
       <c r="C5" s="51" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D5" s="51" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E5" s="52">
         <v>4</v>
@@ -2470,7 +2465,7 @@
         <v>0.1</v>
       </c>
       <c r="I5" s="51" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="J5" s="51"/>
     </row>
@@ -2482,10 +2477,10 @@
         <v>3001</v>
       </c>
       <c r="C6" s="51" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D6" s="51" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E6" s="52">
         <v>5</v>
@@ -2500,7 +2495,7 @@
         <v>0.1</v>
       </c>
       <c r="I6" s="51" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="J6" s="51"/>
     </row>
@@ -2512,10 +2507,10 @@
         <v>3002</v>
       </c>
       <c r="C7" s="51" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D7" s="51" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E7" s="52">
         <v>6</v>
@@ -2530,7 +2525,7 @@
         <v>0.02</v>
       </c>
       <c r="I7" s="51" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="J7" s="51"/>
     </row>
@@ -2556,52 +2551,52 @@
         <v>15</v>
       </c>
       <c r="B1" s="43" t="s">
+        <v>178</v>
+      </c>
+      <c r="C1" s="43" t="s">
+        <v>179</v>
+      </c>
+      <c r="D1" s="43" t="s">
+        <v>180</v>
+      </c>
+      <c r="E1" s="43" t="s">
+        <v>181</v>
+      </c>
+      <c r="F1" s="43" t="s">
+        <v>182</v>
+      </c>
+      <c r="G1" s="43" t="s">
+        <v>183</v>
+      </c>
+      <c r="H1" s="43" t="s">
+        <v>184</v>
+      </c>
+      <c r="I1" s="43" t="s">
+        <v>185</v>
+      </c>
+      <c r="J1" s="43" t="s">
         <v>186</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="K1" s="43" t="s">
         <v>187</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="L1" s="43" t="s">
         <v>188</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="M1" s="43" t="s">
         <v>189</v>
       </c>
-      <c r="F1" s="43" t="s">
+      <c r="N1" s="43" t="s">
         <v>190</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="O1" s="43" t="s">
         <v>191</v>
       </c>
-      <c r="H1" s="43" t="s">
+      <c r="P1" s="43" t="s">
         <v>192</v>
       </c>
-      <c r="I1" s="43" t="s">
+      <c r="Q1" s="43" t="s">
         <v>193</v>
-      </c>
-      <c r="J1" s="43" t="s">
-        <v>194</v>
-      </c>
-      <c r="K1" s="43" t="s">
-        <v>195</v>
-      </c>
-      <c r="L1" s="43" t="s">
-        <v>196</v>
-      </c>
-      <c r="M1" s="43" t="s">
-        <v>197</v>
-      </c>
-      <c r="N1" s="43" t="s">
-        <v>198</v>
-      </c>
-      <c r="O1" s="43" t="s">
-        <v>199</v>
-      </c>
-      <c r="P1" s="43" t="s">
-        <v>200</v>
-      </c>
-      <c r="Q1" s="43" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="17.5" thickBot="1">
@@ -2612,7 +2607,7 @@
         <v>3000</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="D2" s="9">
         <v>0</v>
@@ -2681,25 +2676,25 @@
         <v>15</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="51.5" thickBot="1">
@@ -2707,16 +2702,16 @@
         <v>100</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="F2" s="6">
         <v>2000</v>
@@ -2725,7 +2720,7 @@
         <v>1000</v>
       </c>
       <c r="H2" s="64" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -2738,7 +2733,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C3195C9-FEDE-4BF4-A7E9-B3000F216BE6}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
@@ -2746,37 +2741,37 @@
   <sheetData>
     <row r="1" spans="1:11" ht="34.5" thickBot="1">
       <c r="A1" s="40" t="s">
+        <v>234</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>236</v>
+      </c>
+      <c r="D1" s="44" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="E1" s="44" t="s">
+        <v>253</v>
+      </c>
+      <c r="F1" s="42" t="s">
         <v>246</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="G1" s="42" t="s">
+        <v>254</v>
+      </c>
+      <c r="H1" s="43" t="s">
         <v>247</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="I1" s="43" t="s">
+        <v>255</v>
+      </c>
+      <c r="J1" s="41" t="s">
+        <v>248</v>
+      </c>
+      <c r="K1" s="47" t="s">
         <v>256</v>
-      </c>
-      <c r="E1" s="44" t="s">
-        <v>264</v>
-      </c>
-      <c r="F1" s="42" t="s">
-        <v>257</v>
-      </c>
-      <c r="G1" s="42" t="s">
-        <v>265</v>
-      </c>
-      <c r="H1" s="43" t="s">
-        <v>258</v>
-      </c>
-      <c r="I1" s="43" t="s">
-        <v>266</v>
-      </c>
-      <c r="J1" s="41" t="s">
-        <v>259</v>
-      </c>
-      <c r="K1" s="47" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="51.5" thickBot="1">
@@ -2790,25 +2785,25 @@
         <v>1000</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="E2" s="9">
         <v>0.3</v>
       </c>
       <c r="F2" s="37" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="G2" s="9">
         <v>0.2</v>
       </c>
       <c r="H2" s="37" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="I2" s="9">
         <v>0.25</v>
       </c>
       <c r="J2" s="37" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="K2" s="9">
         <v>0.25</v>
@@ -2873,25 +2868,25 @@
         <v>23</v>
       </c>
       <c r="J1" s="57" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="K1" s="58" t="s">
         <v>24</v>
       </c>
       <c r="L1" s="58" t="s">
+        <v>101</v>
+      </c>
+      <c r="M1" s="58" t="s">
         <v>104</v>
       </c>
-      <c r="M1" s="58" t="s">
-        <v>107</v>
-      </c>
       <c r="N1" s="45" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="O1" s="45" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="P1" s="45" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="34.5" thickBot="1">
@@ -2962,7 +2957,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="37" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="H3" s="37" t="s">
         <v>28</v>
@@ -3010,7 +3005,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="61" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="H4" s="61" t="s">
         <v>29</v>
@@ -3058,10 +3053,10 @@
         <v>2</v>
       </c>
       <c r="G5" s="37" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="H5" s="37" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="I5" s="38" t="b">
         <v>0</v>
@@ -3106,10 +3101,10 @@
         <v>1</v>
       </c>
       <c r="G6" s="37" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="H6" s="37" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="I6" s="38" t="b">
         <v>0</v>
@@ -3154,7 +3149,7 @@
         <v>2</v>
       </c>
       <c r="G7" s="37" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="H7" s="37" t="s">
         <v>31</v>
@@ -3204,7 +3199,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="37" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="H8" s="37" t="s">
         <v>32</v>
@@ -3231,7 +3226,7 @@
         <v>0</v>
       </c>
       <c r="P8" s="37" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="17.5" thickBot="1">
@@ -3254,7 +3249,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="37" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="H9" s="37" t="s">
         <v>33</v>
@@ -3281,7 +3276,7 @@
         <v>0</v>
       </c>
       <c r="P9" s="37" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="17.5" thickBot="1">
@@ -3304,7 +3299,7 @@
         <v>3</v>
       </c>
       <c r="G10" s="37" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="H10" s="37" t="s">
         <v>34</v>
@@ -3331,7 +3326,7 @@
         <v>0</v>
       </c>
       <c r="P10" s="37" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="34.5" thickBot="1">
@@ -3354,7 +3349,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="37" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="H11" s="37" t="s">
         <v>35</v>
@@ -3381,7 +3376,7 @@
         <v>2000</v>
       </c>
       <c r="P11" s="37" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="17.5" thickBot="1">
@@ -3404,7 +3399,7 @@
         <v>2</v>
       </c>
       <c r="G12" s="37" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="H12" s="37" t="s">
         <v>36</v>
@@ -3454,7 +3449,7 @@
         <v>1</v>
       </c>
       <c r="G13" s="63" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="H13" s="37" t="s">
         <v>38</v>
@@ -3504,7 +3499,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="37" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="H14" s="37" t="s">
         <v>39</v>
@@ -3531,7 +3526,7 @@
         <v>0</v>
       </c>
       <c r="P14" s="37" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="17.5" thickBot="1">
@@ -3554,7 +3549,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="37" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="H15" s="37" t="s">
         <v>40</v>
@@ -3581,7 +3576,7 @@
         <v>0</v>
       </c>
       <c r="P15" s="63" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="34.5" thickBot="1">
@@ -3604,7 +3599,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="37" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="H16" s="37" t="s">
         <v>41</v>
@@ -3631,7 +3626,7 @@
         <v>0</v>
       </c>
       <c r="P16" s="37" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="34.5" thickBot="1">
@@ -3654,7 +3649,7 @@
         <v>1</v>
       </c>
       <c r="G17" s="37" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="H17" s="37" t="s">
         <v>42</v>
@@ -3681,7 +3676,7 @@
         <v>3002</v>
       </c>
       <c r="P17" s="37" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -5109,7 +5104,7 @@
         <v>103012101</v>
       </c>
       <c r="B29" s="37" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C29" s="9">
         <v>1</v>
@@ -5209,7 +5204,7 @@
         <v>103012103</v>
       </c>
       <c r="B31" s="37" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C31" s="9">
         <v>1</v>
@@ -5259,7 +5254,7 @@
         <v>103012104</v>
       </c>
       <c r="B32" s="37" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C32" s="9">
         <v>1</v>
@@ -5309,7 +5304,7 @@
         <v>103012201</v>
       </c>
       <c r="B33" s="37" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C33" s="9">
         <v>2</v>
@@ -5409,7 +5404,7 @@
         <v>103012203</v>
       </c>
       <c r="B35" s="37" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C35" s="9">
         <v>2</v>
@@ -5459,7 +5454,7 @@
         <v>103012204</v>
       </c>
       <c r="B36" s="37" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C36" s="9">
         <v>2</v>
@@ -5509,7 +5504,7 @@
         <v>103012301</v>
       </c>
       <c r="B37" s="37" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C37" s="9">
         <v>3</v>
@@ -5609,7 +5604,7 @@
         <v>103012303</v>
       </c>
       <c r="B39" s="37" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C39" s="9">
         <v>3</v>
@@ -5659,7 +5654,7 @@
         <v>103012304</v>
       </c>
       <c r="B40" s="37" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C40" s="9">
         <v>3</v>
@@ -5709,7 +5704,7 @@
         <v>103012401</v>
       </c>
       <c r="B41" s="37" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C41" s="9">
         <v>4</v>
@@ -5809,7 +5804,7 @@
         <v>103012403</v>
       </c>
       <c r="B43" s="37" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C43" s="9">
         <v>4</v>
@@ -5859,7 +5854,7 @@
         <v>103012404</v>
       </c>
       <c r="B44" s="37" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C44" s="9">
         <v>4</v>
@@ -5909,7 +5904,7 @@
         <v>103012501</v>
       </c>
       <c r="B45" s="37" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C45" s="9">
         <v>5</v>
@@ -6009,7 +6004,7 @@
         <v>103012503</v>
       </c>
       <c r="B47" s="37" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C47" s="9">
         <v>5</v>
@@ -6059,7 +6054,7 @@
         <v>103012504</v>
       </c>
       <c r="B48" s="37" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C48" s="9">
         <v>5</v>
@@ -11154,10 +11149,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C931ABBA-9A51-4E37-A8BC-ACBFBA422EE1}">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="17"/>
@@ -11172,7 +11167,7 @@
     <col min="12" max="16384" width="8.58203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="34.5" thickBot="1">
+    <row r="1" spans="1:18" ht="34.5" thickBot="1">
       <c r="A1" s="10" t="s">
         <v>15</v>
       </c>
@@ -11222,10 +11217,13 @@
         <v>84</v>
       </c>
       <c r="Q1" s="14" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="17.5" thickBot="1">
+        <v>207</v>
+      </c>
+      <c r="R1" s="18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="51.5" thickBot="1">
       <c r="A2" s="6">
         <v>1000</v>
       </c>
@@ -11236,7 +11234,7 @@
         <v>30</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>85</v>
+        <v>259</v>
       </c>
       <c r="E2" s="6" t="b">
         <v>1</v>
@@ -11277,8 +11275,11 @@
       <c r="Q2" s="17">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" ht="17.5" thickBot="1">
+      <c r="R2" s="37" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="51.5" thickBot="1">
       <c r="A3" s="6">
         <v>2000</v>
       </c>
@@ -11289,7 +11290,7 @@
         <v>20</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>86</v>
+        <v>260</v>
       </c>
       <c r="E3" s="6" t="b">
         <v>0</v>
@@ -11330,8 +11331,11 @@
       <c r="Q3" s="17">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" ht="17.5" thickBot="1">
+      <c r="R3" s="37" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="17.5" thickBot="1">
       <c r="A4" s="6">
         <v>3000</v>
       </c>
@@ -11342,7 +11346,7 @@
         <v>15</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>87</v>
+        <v>261</v>
       </c>
       <c r="E4" s="6" t="b">
         <v>0</v>
@@ -11383,8 +11387,11 @@
       <c r="Q4" s="56">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" ht="17.5" thickBot="1">
+      <c r="R4" s="63" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="17.5" thickBot="1">
       <c r="A5" s="6"/>
     </row>
   </sheetData>
@@ -11405,46 +11412,46 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" t="s">
         <v>126</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>127</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>128</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J1" t="s">
         <v>129</v>
       </c>
-      <c r="E1" t="s">
+      <c r="K1" t="s">
         <v>130</v>
       </c>
-      <c r="F1" t="s">
+      <c r="L1" t="s">
         <v>131</v>
       </c>
-      <c r="G1" t="s">
-        <v>136</v>
-      </c>
-      <c r="H1" t="s">
-        <v>137</v>
-      </c>
-      <c r="I1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>132</v>
       </c>
-      <c r="K1" t="s">
-        <v>133</v>
-      </c>
-      <c r="L1" t="s">
-        <v>134</v>
-      </c>
-      <c r="M1" t="s">
-        <v>135</v>
-      </c>
       <c r="N1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -11499,10 +11506,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B4BE54-90AE-4DAF-BA80-4CA3867A9D82}">
-  <dimension ref="A1:AM12"/>
+  <dimension ref="A1:AM11"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8:U11"/>
+    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="17"/>
@@ -11515,19 +11522,19 @@
         <v>15</v>
       </c>
       <c r="B1" s="40" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C1" s="45" t="s">
         <v>17</v>
       </c>
       <c r="D1" s="45" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E1" s="44" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F1" s="44" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G1" s="42" t="s">
         <v>76</v>
@@ -11536,7 +11543,7 @@
         <v>77</v>
       </c>
       <c r="I1" s="42" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J1" s="42" t="s">
         <v>79</v>
@@ -11548,37 +11555,37 @@
         <v>81</v>
       </c>
       <c r="M1" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="N1" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="O1" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="P1" s="41" t="s">
         <v>91</v>
       </c>
-      <c r="N1" s="41" t="s">
+      <c r="Q1" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="O1" s="41" t="s">
+      <c r="R1" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="P1" s="41" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q1" s="41" t="s">
-        <v>95</v>
-      </c>
-      <c r="R1" s="41" t="s">
-        <v>96</v>
-      </c>
       <c r="S1" s="43" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="T1" s="47" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="U1" s="53" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="V1" s="43" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="W1" s="43" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="X1" s="43"/>
       <c r="Y1" s="43"/>
@@ -11602,13 +11609,13 @@
         <v>1000</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C2" s="9">
         <v>1</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E2" s="9">
         <v>150</v>
@@ -11689,13 +11696,13 @@
         <v>1001</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C3" s="9">
         <v>1</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E3" s="9">
         <v>200</v>
@@ -11773,25 +11780,25 @@
     </row>
     <row r="4" spans="1:39" ht="34.5" thickBot="1">
       <c r="A4" s="9">
-        <v>1002</v>
+        <v>2000</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>166</v>
+        <v>98</v>
       </c>
       <c r="C4" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E4" s="9">
-        <v>250</v>
+        <v>700</v>
       </c>
       <c r="F4" s="9">
         <v>5</v>
       </c>
       <c r="G4" s="9">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H4" s="9">
         <v>0</v>
@@ -11809,7 +11816,7 @@
         <v>0</v>
       </c>
       <c r="M4" s="9">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="N4" s="9">
         <v>0</v>
@@ -11833,7 +11840,7 @@
         <v>0</v>
       </c>
       <c r="U4" s="9">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="V4" s="54">
         <v>0</v>
@@ -11860,25 +11867,25 @@
     </row>
     <row r="5" spans="1:39" ht="34.5" thickBot="1">
       <c r="A5" s="9">
-        <v>2000</v>
+        <v>2001</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>101</v>
+        <v>163</v>
       </c>
       <c r="C5" s="9">
         <v>2</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E5" s="9">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="F5" s="9">
         <v>5</v>
       </c>
       <c r="G5" s="9">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H5" s="9">
         <v>0</v>
@@ -11920,7 +11927,7 @@
         <v>0</v>
       </c>
       <c r="U5" s="9">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="V5" s="54">
         <v>0</v>
@@ -11947,25 +11954,25 @@
     </row>
     <row r="6" spans="1:39" ht="34.5" thickBot="1">
       <c r="A6" s="9">
-        <v>2001</v>
+        <v>3000</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="C6" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>102</v>
+        <v>173</v>
       </c>
       <c r="E6" s="9">
-        <v>800</v>
+        <v>4000</v>
       </c>
       <c r="F6" s="9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G6" s="9">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="H6" s="9">
         <v>0</v>
@@ -11983,37 +11990,37 @@
         <v>0</v>
       </c>
       <c r="M6" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="N6" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="O6" s="9">
+        <v>0</v>
+      </c>
+      <c r="P6" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="Q6" s="9">
+        <v>0</v>
+      </c>
+      <c r="R6" s="9">
+        <v>0</v>
+      </c>
+      <c r="S6" s="54">
+        <v>0</v>
+      </c>
+      <c r="T6" s="54">
+        <v>0</v>
+      </c>
+      <c r="U6" s="9">
+        <v>5000</v>
+      </c>
+      <c r="V6" s="9">
+        <v>3000</v>
+      </c>
+      <c r="W6" s="9">
         <v>0.2</v>
-      </c>
-      <c r="N6" s="9">
-        <v>0</v>
-      </c>
-      <c r="O6" s="9">
-        <v>0</v>
-      </c>
-      <c r="P6" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="9">
-        <v>0</v>
-      </c>
-      <c r="R6" s="9">
-        <v>0</v>
-      </c>
-      <c r="S6" s="9">
-        <v>0</v>
-      </c>
-      <c r="T6" s="9">
-        <v>0</v>
-      </c>
-      <c r="U6" s="9">
-        <v>80</v>
-      </c>
-      <c r="V6" s="54">
-        <v>0</v>
-      </c>
-      <c r="W6" s="54">
-        <v>0</v>
       </c>
       <c r="X6" s="9"/>
       <c r="Y6" s="37"/>
@@ -12034,25 +12041,25 @@
     </row>
     <row r="7" spans="1:39" ht="34.5" thickBot="1">
       <c r="A7" s="9">
-        <v>2002</v>
+        <v>4000</v>
       </c>
       <c r="B7" s="37" t="s">
         <v>176</v>
       </c>
       <c r="C7" s="9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>102</v>
+        <v>177</v>
       </c>
       <c r="E7" s="9">
-        <v>900</v>
+        <v>15000</v>
       </c>
       <c r="F7" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G7" s="9">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="H7" s="9">
         <v>0</v>
@@ -12088,19 +12095,19 @@
         <v>0</v>
       </c>
       <c r="S7" s="9">
-        <v>0</v>
+        <v>7500</v>
       </c>
       <c r="T7" s="9">
         <v>0</v>
       </c>
-      <c r="U7" s="9">
-        <v>120</v>
-      </c>
-      <c r="V7" s="54">
-        <v>0</v>
-      </c>
-      <c r="W7" s="54">
-        <v>0</v>
+      <c r="U7" s="54">
+        <v>0</v>
+      </c>
+      <c r="V7" s="9">
+        <v>7000</v>
+      </c>
+      <c r="W7" s="9">
+        <v>0.33</v>
       </c>
       <c r="X7" s="9"/>
       <c r="Y7" s="37"/>
@@ -12119,76 +12126,7 @@
       <c r="AL7" s="9"/>
       <c r="AM7" s="37"/>
     </row>
-    <row r="8" spans="1:39" ht="34.5" thickBot="1">
-      <c r="A8" s="9">
-        <v>3000</v>
-      </c>
-      <c r="B8" s="37" t="s">
-        <v>177</v>
-      </c>
-      <c r="C8" s="9">
-        <v>3</v>
-      </c>
-      <c r="D8" s="37" t="s">
-        <v>178</v>
-      </c>
-      <c r="E8" s="9">
-        <v>4000</v>
-      </c>
-      <c r="F8" s="9">
-        <v>6</v>
-      </c>
-      <c r="G8" s="9">
-        <v>40</v>
-      </c>
-      <c r="H8" s="9">
-        <v>0</v>
-      </c>
-      <c r="I8" s="9">
-        <v>0</v>
-      </c>
-      <c r="J8" s="9">
-        <v>0</v>
-      </c>
-      <c r="K8" s="9">
-        <v>0</v>
-      </c>
-      <c r="L8" s="9">
-        <v>0</v>
-      </c>
-      <c r="M8" s="9">
-        <v>0.4</v>
-      </c>
-      <c r="N8" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="O8" s="9">
-        <v>0</v>
-      </c>
-      <c r="P8" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="Q8" s="9">
-        <v>0</v>
-      </c>
-      <c r="R8" s="9">
-        <v>0</v>
-      </c>
-      <c r="S8" s="54">
-        <v>0</v>
-      </c>
-      <c r="T8" s="54">
-        <v>0</v>
-      </c>
-      <c r="U8" s="9">
-        <v>5000</v>
-      </c>
-      <c r="V8" s="9">
-        <v>3000</v>
-      </c>
-      <c r="W8" s="9">
-        <v>0.2</v>
-      </c>
+    <row r="8" spans="1:39" ht="17.5" thickBot="1">
       <c r="X8" s="9"/>
       <c r="Y8" s="37"/>
       <c r="Z8" s="9"/>
@@ -12206,77 +12144,7 @@
       <c r="AL8" s="9"/>
       <c r="AM8" s="37"/>
     </row>
-    <row r="9" spans="1:39" ht="34.5" thickBot="1">
-      <c r="A9" s="9">
-        <v>3001</v>
-      </c>
-      <c r="B9" s="37" t="s">
-        <v>179</v>
-      </c>
-      <c r="C9" s="9">
-        <v>3</v>
-      </c>
-      <c r="D9" s="37" t="s">
-        <v>178</v>
-      </c>
-      <c r="E9" s="9">
-        <v>8000</v>
-      </c>
-      <c r="F9" s="9">
-        <v>6</v>
-      </c>
-      <c r="G9" s="9">
-        <v>65</v>
-      </c>
-      <c r="H9" s="9">
-        <v>0</v>
-      </c>
-      <c r="I9" s="9">
-        <v>0</v>
-      </c>
-      <c r="J9" s="9">
-        <v>0</v>
-      </c>
-      <c r="K9" s="9">
-        <v>0</v>
-      </c>
-      <c r="L9" s="9">
-        <v>0</v>
-      </c>
-      <c r="M9" s="9">
-        <v>0.4</v>
-      </c>
-      <c r="N9" s="9">
-        <v>0</v>
-      </c>
-      <c r="O9" s="9">
-        <v>0</v>
-      </c>
-      <c r="P9" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="9">
-        <v>0</v>
-      </c>
-      <c r="R9" s="9">
-        <v>0</v>
-      </c>
-      <c r="S9" s="54">
-        <v>0</v>
-      </c>
-      <c r="T9" s="54">
-        <v>0</v>
-      </c>
-      <c r="U9" s="9">
-        <v>7000</v>
-      </c>
-      <c r="V9" s="9">
-        <v>6000</v>
-      </c>
-      <c r="W9" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="X9" s="9"/>
+    <row r="9" spans="1:39" ht="17.5" thickBot="1">
       <c r="Y9" s="37"/>
       <c r="Z9" s="9"/>
       <c r="AA9" s="37"/>
@@ -12293,77 +12161,7 @@
       <c r="AL9" s="9"/>
       <c r="AM9" s="37"/>
     </row>
-    <row r="10" spans="1:39" ht="34.5" thickBot="1">
-      <c r="A10" s="9">
-        <v>3002</v>
-      </c>
-      <c r="B10" s="37" t="s">
-        <v>180</v>
-      </c>
-      <c r="C10" s="9">
-        <v>3</v>
-      </c>
-      <c r="D10" s="37" t="s">
-        <v>178</v>
-      </c>
-      <c r="E10" s="9">
-        <v>5000</v>
-      </c>
-      <c r="F10" s="9">
-        <v>6</v>
-      </c>
-      <c r="G10" s="9">
-        <v>50</v>
-      </c>
-      <c r="H10" s="9">
-        <v>0</v>
-      </c>
-      <c r="I10" s="9">
-        <v>0</v>
-      </c>
-      <c r="J10" s="9">
-        <v>0</v>
-      </c>
-      <c r="K10" s="9">
-        <v>0</v>
-      </c>
-      <c r="L10" s="9">
-        <v>0</v>
-      </c>
-      <c r="M10" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="N10" s="9">
-        <v>0</v>
-      </c>
-      <c r="O10" s="9">
-        <v>0</v>
-      </c>
-      <c r="P10" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="9">
-        <v>0</v>
-      </c>
-      <c r="R10" s="9">
-        <v>0</v>
-      </c>
-      <c r="S10" s="54">
-        <v>0</v>
-      </c>
-      <c r="T10" s="54">
-        <v>0</v>
-      </c>
-      <c r="U10" s="9">
-        <v>5000</v>
-      </c>
-      <c r="V10" s="9">
-        <v>2000</v>
-      </c>
-      <c r="W10" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="X10" s="9"/>
+    <row r="10" spans="1:39" ht="17.5" thickBot="1">
       <c r="Y10" s="37"/>
       <c r="Z10" s="9"/>
       <c r="AA10" s="37"/>
@@ -12380,80 +12178,7 @@
       <c r="AL10" s="9"/>
       <c r="AM10" s="37"/>
     </row>
-    <row r="11" spans="1:39" ht="34.5" thickBot="1">
-      <c r="A11" s="9">
-        <v>3003</v>
-      </c>
-      <c r="B11" s="37" t="s">
-        <v>181</v>
-      </c>
-      <c r="C11" s="9">
-        <v>3</v>
-      </c>
-      <c r="D11" s="37" t="s">
-        <v>178</v>
-      </c>
-      <c r="E11" s="9">
-        <v>10000</v>
-      </c>
-      <c r="F11" s="9">
-        <v>6</v>
-      </c>
-      <c r="G11" s="9">
-        <v>85</v>
-      </c>
-      <c r="H11" s="9">
-        <v>0</v>
-      </c>
-      <c r="I11" s="9">
-        <v>0</v>
-      </c>
-      <c r="J11" s="9">
-        <v>0</v>
-      </c>
-      <c r="K11" s="9">
-        <v>0</v>
-      </c>
-      <c r="L11" s="9">
-        <v>0</v>
-      </c>
-      <c r="M11" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="N11" s="9">
-        <v>0</v>
-      </c>
-      <c r="O11" s="9">
-        <v>0</v>
-      </c>
-      <c r="P11" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="9">
-        <v>0</v>
-      </c>
-      <c r="R11" s="9">
-        <v>0</v>
-      </c>
-      <c r="S11" s="54">
-        <v>0</v>
-      </c>
-      <c r="T11" s="54">
-        <v>0</v>
-      </c>
-      <c r="U11" s="9">
-        <v>7000</v>
-      </c>
-      <c r="V11" s="9">
-        <v>4000</v>
-      </c>
-      <c r="W11" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="X11" s="9"/>
-      <c r="Y11" s="37"/>
-      <c r="Z11" s="9"/>
-      <c r="AA11" s="37"/>
+    <row r="11" spans="1:39" ht="17.5" thickBot="1">
       <c r="AB11" s="9"/>
       <c r="AC11" s="37"/>
       <c r="AD11" s="9"/>
@@ -12467,93 +12192,6 @@
       <c r="AL11" s="9"/>
       <c r="AM11" s="37"/>
     </row>
-    <row r="12" spans="1:39" ht="34.5" thickBot="1">
-      <c r="A12" s="9">
-        <v>4000</v>
-      </c>
-      <c r="B12" s="37" t="s">
-        <v>184</v>
-      </c>
-      <c r="C12" s="9">
-        <v>4</v>
-      </c>
-      <c r="D12" s="37" t="s">
-        <v>185</v>
-      </c>
-      <c r="E12" s="9">
-        <v>15000</v>
-      </c>
-      <c r="F12" s="9">
-        <v>0</v>
-      </c>
-      <c r="G12" s="9">
-        <v>100</v>
-      </c>
-      <c r="H12" s="9">
-        <v>0</v>
-      </c>
-      <c r="I12" s="9">
-        <v>0</v>
-      </c>
-      <c r="J12" s="9">
-        <v>0</v>
-      </c>
-      <c r="K12" s="9">
-        <v>0</v>
-      </c>
-      <c r="L12" s="9">
-        <v>0</v>
-      </c>
-      <c r="M12" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="N12" s="9">
-        <v>0</v>
-      </c>
-      <c r="O12" s="9">
-        <v>0</v>
-      </c>
-      <c r="P12" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="9">
-        <v>0</v>
-      </c>
-      <c r="R12" s="9">
-        <v>0</v>
-      </c>
-      <c r="S12" s="9">
-        <v>7500</v>
-      </c>
-      <c r="T12" s="9">
-        <v>0</v>
-      </c>
-      <c r="U12" s="54">
-        <v>0</v>
-      </c>
-      <c r="V12" s="9">
-        <v>7000</v>
-      </c>
-      <c r="W12" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="X12" s="9"/>
-      <c r="Y12" s="37"/>
-      <c r="Z12" s="9"/>
-      <c r="AA12" s="37"/>
-      <c r="AB12" s="9"/>
-      <c r="AC12" s="37"/>
-      <c r="AD12" s="9"/>
-      <c r="AE12" s="37"/>
-      <c r="AF12" s="9"/>
-      <c r="AG12" s="37"/>
-      <c r="AH12" s="9"/>
-      <c r="AI12" s="37"/>
-      <c r="AJ12" s="9"/>
-      <c r="AK12" s="37"/>
-      <c r="AL12" s="9"/>
-      <c r="AM12" s="37"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12566,7 +12204,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17"/>
@@ -12581,39 +12219,39 @@
         <v>15</v>
       </c>
       <c r="B1" s="40" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="42" t="s">
         <v>114</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="F1" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="G1" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="E1" s="42" t="s">
-        <v>117</v>
-      </c>
-      <c r="F1" s="43" t="s">
-        <v>118</v>
-      </c>
-      <c r="G1" s="43" t="s">
-        <v>119</v>
-      </c>
       <c r="H1" s="43" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I1" s="43" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="J1" s="44" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="51.5" thickBot="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="34.5" thickBot="1">
       <c r="A2" s="9">
         <v>100000</v>
       </c>
-      <c r="B2" s="37" t="s">
-        <v>204</v>
+      <c r="B2" s="39" t="s">
+        <v>257</v>
       </c>
       <c r="C2" s="9">
         <v>1</v>
@@ -12637,15 +12275,15 @@
         <v>0</v>
       </c>
       <c r="J2" s="37" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="51.5" thickBot="1">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="29.5" thickBot="1">
       <c r="A3" s="9">
         <v>200000</v>
       </c>
-      <c r="B3" s="37" t="s">
-        <v>205</v>
+      <c r="B3" s="39" t="s">
+        <v>258</v>
       </c>
       <c r="C3" s="9">
         <v>1</v>
@@ -12669,15 +12307,15 @@
         <v>0</v>
       </c>
       <c r="J3" s="37" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="34.5" thickBot="1">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="17.5" thickBot="1">
       <c r="A4" s="9">
         <v>300000</v>
       </c>
-      <c r="B4" s="37" t="s">
-        <v>206</v>
+      <c r="B4" s="1">
+        <v>3000</v>
       </c>
       <c r="C4" s="9">
         <v>2</v>
@@ -12701,15 +12339,15 @@
         <v>0</v>
       </c>
       <c r="J4" s="37" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="34.5" thickBot="1">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="17.5" thickBot="1">
       <c r="A5" s="9">
         <v>300001</v>
       </c>
-      <c r="B5" s="37" t="s">
-        <v>206</v>
+      <c r="B5" s="1">
+        <v>3000</v>
       </c>
       <c r="C5" s="9">
         <v>4</v>
@@ -12733,15 +12371,15 @@
         <v>0</v>
       </c>
       <c r="J5" s="37" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="34.5" thickBot="1">
       <c r="A6" s="9">
         <v>300002</v>
       </c>
-      <c r="B6" s="37" t="s">
-        <v>206</v>
+      <c r="B6" s="1">
+        <v>3000</v>
       </c>
       <c r="C6" s="9">
         <v>4</v>
@@ -12765,15 +12403,15 @@
         <v>0</v>
       </c>
       <c r="J6" s="37" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="34.5" thickBot="1">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="17.5" thickBot="1">
       <c r="A7" s="9">
         <v>300003</v>
       </c>
-      <c r="B7" s="37" t="s">
-        <v>206</v>
+      <c r="B7" s="1">
+        <v>3000</v>
       </c>
       <c r="C7" s="9">
         <v>4</v>
@@ -12797,15 +12435,15 @@
         <v>0</v>
       </c>
       <c r="J7" s="37" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="34.5" thickBot="1">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="17.5" thickBot="1">
       <c r="A8" s="9">
         <v>300004</v>
       </c>
-      <c r="B8" s="37" t="s">
-        <v>206</v>
+      <c r="B8" s="1">
+        <v>3000</v>
       </c>
       <c r="C8" s="9">
         <v>3</v>
@@ -12829,15 +12467,15 @@
         <v>0</v>
       </c>
       <c r="J8" s="37" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="34.5" thickBot="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="17.5" thickBot="1">
       <c r="A9" s="9">
         <v>300005</v>
       </c>
-      <c r="B9" s="37" t="s">
-        <v>206</v>
+      <c r="B9" s="1">
+        <v>3000</v>
       </c>
       <c r="C9" s="9">
         <v>1</v>
@@ -12861,15 +12499,15 @@
         <v>0</v>
       </c>
       <c r="J9" s="37" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="34.5" thickBot="1">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="17.5" thickBot="1">
       <c r="A10" s="9">
         <v>300006</v>
       </c>
-      <c r="B10" s="37" t="s">
-        <v>206</v>
+      <c r="B10" s="1">
+        <v>3000</v>
       </c>
       <c r="C10" s="9">
         <v>1</v>
@@ -12893,15 +12531,15 @@
         <v>0</v>
       </c>
       <c r="J10" s="37" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="34.5" thickBot="1">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="17.5" thickBot="1">
       <c r="A11" s="9">
         <v>300008</v>
       </c>
-      <c r="B11" s="37" t="s">
-        <v>206</v>
+      <c r="B11" s="1">
+        <v>3000</v>
       </c>
       <c r="C11" s="9">
         <v>1</v>
@@ -12925,15 +12563,15 @@
         <v>0</v>
       </c>
       <c r="J11" s="37" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="34.5" thickBot="1">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="17.5" thickBot="1">
       <c r="A12" s="9">
         <v>300009</v>
       </c>
-      <c r="B12" s="37" t="s">
-        <v>206</v>
+      <c r="B12" s="1">
+        <v>3000</v>
       </c>
       <c r="C12" s="9">
         <v>2</v>
@@ -12957,15 +12595,15 @@
         <v>0</v>
       </c>
       <c r="J12" s="37" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="34.5" thickBot="1">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="17.5" thickBot="1">
       <c r="A13" s="9">
         <v>300010</v>
       </c>
-      <c r="B13" s="37" t="s">
-        <v>206</v>
+      <c r="B13" s="1">
+        <v>3000</v>
       </c>
       <c r="C13" s="9">
         <v>5</v>
@@ -12989,15 +12627,15 @@
         <v>0</v>
       </c>
       <c r="J13" s="37" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="34.5" thickBot="1">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="17.5" thickBot="1">
       <c r="A14" s="9">
         <v>300011</v>
       </c>
-      <c r="B14" s="37" t="s">
-        <v>206</v>
+      <c r="B14" s="1">
+        <v>3000</v>
       </c>
       <c r="C14" s="9">
         <v>3</v>
@@ -13021,7 +12659,7 @@
         <v>0</v>
       </c>
       <c r="J14" s="37" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -13052,40 +12690,40 @@
         <v>15</v>
       </c>
       <c r="B1" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="I1" s="46" t="s">
+        <v>118</v>
+      </c>
+      <c r="J1" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="K1" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="C1" s="42" t="s">
-        <v>143</v>
-      </c>
-      <c r="D1" s="42" t="s">
-        <v>142</v>
-      </c>
-      <c r="E1" s="42" t="s">
-        <v>141</v>
-      </c>
-      <c r="F1" s="42" t="s">
-        <v>140</v>
-      </c>
-      <c r="G1" s="42" t="s">
-        <v>138</v>
-      </c>
-      <c r="H1" s="42" t="s">
-        <v>139</v>
-      </c>
-      <c r="I1" s="46" t="s">
+      <c r="L1" s="41" t="s">
         <v>121</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="M1" s="47" t="s">
         <v>122</v>
-      </c>
-      <c r="K1" s="41" t="s">
-        <v>123</v>
-      </c>
-      <c r="L1" s="41" t="s">
-        <v>124</v>
-      </c>
-      <c r="M1" s="47" t="s">
-        <v>125</v>
       </c>
       <c r="N1" s="18"/>
     </row>
@@ -13094,7 +12732,7 @@
         <v>1000001</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C2" s="9">
         <v>1</v>
@@ -13136,7 +12774,7 @@
         <v>2000001</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C3" s="9">
         <v>1</v>
@@ -13178,7 +12816,7 @@
         <v>3000001</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C4" s="9">
         <v>1</v>
@@ -13219,7 +12857,7 @@
         <v>3000002</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C5" s="9">
         <v>1</v>
@@ -13260,7 +12898,7 @@
         <v>3000011</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C6" s="9">
         <v>1</v>
@@ -13301,7 +12939,7 @@
         <v>3000012</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C7" s="9">
         <v>1</v>
@@ -13342,7 +12980,7 @@
         <v>3000013</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C8" s="9">
         <v>2</v>
@@ -13383,7 +13021,7 @@
         <v>3000014</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C9" s="9">
         <v>1.5</v>
@@ -13424,7 +13062,7 @@
         <v>3000021</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C10" s="9">
         <v>1</v>
@@ -13465,7 +13103,7 @@
         <v>3000022</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C11" s="9">
         <v>1</v>
@@ -13506,7 +13144,7 @@
         <v>3000023</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C12" s="9">
         <v>1</v>
@@ -13547,7 +13185,7 @@
         <v>3000024</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C13" s="9">
         <v>1</v>
@@ -13588,7 +13226,7 @@
         <v>3000031</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C14" s="9">
         <v>1</v>
@@ -13629,7 +13267,7 @@
         <v>3000032</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C15" s="9">
         <v>1</v>
@@ -13670,7 +13308,7 @@
         <v>3000033</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C16" s="9">
         <v>1</v>
@@ -13711,7 +13349,7 @@
         <v>3000034</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C17" s="9">
         <v>1.5</v>
@@ -13752,7 +13390,7 @@
         <v>3000041</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C18" s="9">
         <v>1</v>
@@ -13793,7 +13431,7 @@
         <v>3000042</v>
       </c>
       <c r="B19" s="37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C19" s="9">
         <v>1</v>
@@ -13834,7 +13472,7 @@
         <v>3000043</v>
       </c>
       <c r="B20" s="37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C20" s="9">
         <v>2.5</v>
@@ -13875,7 +13513,7 @@
         <v>3000051</v>
       </c>
       <c r="B21" s="37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C21" s="9">
         <v>0.8</v>
@@ -13916,7 +13554,7 @@
         <v>3000061</v>
       </c>
       <c r="B22" s="37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C22" s="9">
         <v>1.2</v>
@@ -13957,7 +13595,7 @@
         <v>3000081</v>
       </c>
       <c r="B23" s="37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C23" s="9">
         <v>2</v>
@@ -13998,7 +13636,7 @@
         <v>3000091</v>
       </c>
       <c r="B24" s="37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C24" s="9">
         <v>2</v>
@@ -14039,7 +13677,7 @@
         <v>3000092</v>
       </c>
       <c r="B25" s="37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C25" s="9">
         <v>1.5</v>
@@ -14080,7 +13718,7 @@
         <v>3000101</v>
       </c>
       <c r="B26" s="37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C26" s="9">
         <v>2</v>
@@ -14121,7 +13759,7 @@
         <v>3000102</v>
       </c>
       <c r="B27" s="37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C27" s="9">
         <v>2</v>
@@ -14162,7 +13800,7 @@
         <v>3000103</v>
       </c>
       <c r="B28" s="37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C28" s="9">
         <v>2</v>
@@ -14203,7 +13841,7 @@
         <v>3000104</v>
       </c>
       <c r="B29" s="37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C29" s="9">
         <v>2</v>
@@ -14244,7 +13882,7 @@
         <v>3000105</v>
       </c>
       <c r="B30" s="37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C30" s="9">
         <v>3</v>
@@ -14285,7 +13923,7 @@
         <v>3000111</v>
       </c>
       <c r="B31" s="37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C31" s="9">
         <v>2.5</v>
@@ -14326,7 +13964,7 @@
         <v>3000112</v>
       </c>
       <c r="B32" s="37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C32" s="9">
         <v>2.5</v>
@@ -14367,7 +14005,7 @@
         <v>3000113</v>
       </c>
       <c r="B33" s="37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C33" s="9">
         <v>3</v>

</xml_diff>